<commit_message>
dev-3.0 : print tanda terima & invoice verification
</commit_message>
<xml_diff>
--- a/storage/template/tandaterima.xlsx
+++ b/storage/template/tandaterima.xlsx
@@ -92,9 +92,6 @@
     <t>Note : Jatuh Tempo</t>
   </si>
   <si>
-    <t>Terbilang    :</t>
-  </si>
-  <si>
     <t>Rev</t>
   </si>
   <si>
@@ -192,13 +189,16 @@
   </si>
   <si>
     <t xml:space="preserve">Supplier </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terbilang </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,12 +273,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Simplified Arabic"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Free "/>
@@ -442,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -489,7 +483,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -511,12 +505,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -550,6 +550,20 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -559,12 +573,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -575,45 +592,19 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -991,7 +982,7 @@
   <dimension ref="A2:O58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:F10"/>
+      <selection activeCell="I5" sqref="I5:N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1032,32 +1023,32 @@
       <c r="J4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="70"/>
+      <c r="M4" s="70"/>
+      <c r="N4" s="70"/>
     </row>
     <row r="5" spans="1:15" ht="17.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="61"/>
-      <c r="J5" s="61"/>
-      <c r="K5" s="61"/>
-      <c r="L5" s="61"/>
-      <c r="M5" s="61"/>
-      <c r="N5" s="61"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="72"/>
+      <c r="N5" s="72"/>
     </row>
     <row r="6" spans="1:15" ht="17.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="61"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="61"/>
-      <c r="L6" s="61"/>
-      <c r="M6" s="61"/>
-      <c r="N6" s="61"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="72"/>
+      <c r="M6" s="72"/>
+      <c r="N6" s="72"/>
     </row>
     <row r="7" spans="1:15" ht="17.25">
       <c r="A7" s="1" t="s">
@@ -1081,15 +1072,15 @@
     </row>
     <row r="9" spans="1:15" ht="17.25">
       <c r="A9" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="35"/>
       <c r="C9" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1099,15 +1090,15 @@
     </row>
     <row r="10" spans="1:15" ht="17.25">
       <c r="A10" s="35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" s="35"/>
       <c r="C10" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1133,27 +1124,27 @@
       <c r="A12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54" t="s">
-        <v>51</v>
-      </c>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54" t="s">
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="64"/>
+      <c r="H12" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="54"/>
-      <c r="J12" s="54"/>
-      <c r="K12" s="54"/>
-      <c r="L12" s="54" t="s">
+      <c r="I12" s="64"/>
+      <c r="J12" s="64"/>
+      <c r="K12" s="64"/>
+      <c r="L12" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="M12" s="54"/>
-      <c r="N12" s="54"/>
+      <c r="M12" s="64"/>
+      <c r="N12" s="64"/>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="34">
@@ -1207,16 +1198,16 @@
     </row>
     <row r="16" spans="1:15" ht="17.25">
       <c r="A16" s="6"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="55"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="55"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
       <c r="L16" s="34"/>
       <c r="M16" s="34"/>
       <c r="N16" s="34"/>
@@ -1239,23 +1230,23 @@
     </row>
     <row r="18" spans="1:14" ht="15.75">
       <c r="A18" s="35" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="B18" s="35"/>
       <c r="C18" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="70"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="70"/>
-      <c r="I18" s="70"/>
-      <c r="J18" s="70"/>
-      <c r="K18" s="70"/>
-      <c r="L18" s="70"/>
-      <c r="M18" s="70"/>
-      <c r="N18" s="70"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="68"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="68"/>
+      <c r="L18" s="68"/>
+      <c r="M18" s="68"/>
+      <c r="N18" s="68"/>
     </row>
     <row r="19" spans="1:14" ht="6.75" customHeight="1">
       <c r="A19" s="1"/>
@@ -1287,10 +1278,10 @@
         <v>17</v>
       </c>
       <c r="J20" s="1"/>
-      <c r="K20" s="59"/>
-      <c r="L20" s="59"/>
-      <c r="M20" s="59"/>
-      <c r="N20" s="59"/>
+      <c r="K20" s="69"/>
+      <c r="L20" s="69"/>
+      <c r="M20" s="69"/>
+      <c r="N20" s="69"/>
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="36"/>
@@ -1299,7 +1290,7 @@
       <c r="D21" s="36"/>
       <c r="E21" s="36"/>
     </row>
-    <row r="22" spans="1:14" ht="20.25">
+    <row r="22" spans="1:14" ht="15.75">
       <c r="A22" s="36"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -1312,12 +1303,12 @@
       <c r="J22" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K22" s="69"/>
-      <c r="L22" s="69"/>
-      <c r="M22" s="69"/>
-      <c r="N22" s="69"/>
-    </row>
-    <row r="23" spans="1:14" ht="20.25">
+      <c r="K22" s="68"/>
+      <c r="L22" s="68"/>
+      <c r="M22" s="68"/>
+      <c r="N22" s="68"/>
+    </row>
+    <row r="23" spans="1:14" ht="15.75">
       <c r="A23" s="36"/>
       <c r="B23" s="36"/>
       <c r="C23" s="36"/>
@@ -1330,12 +1321,12 @@
       <c r="J23" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K23" s="69"/>
-      <c r="L23" s="69"/>
-      <c r="M23" s="69"/>
-      <c r="N23" s="69"/>
-    </row>
-    <row r="24" spans="1:14" ht="20.25">
+      <c r="K23" s="68"/>
+      <c r="L23" s="68"/>
+      <c r="M23" s="68"/>
+      <c r="N23" s="68"/>
+    </row>
+    <row r="24" spans="1:14" ht="15.75">
       <c r="A24" s="36"/>
       <c r="B24" s="36"/>
       <c r="C24" s="36"/>
@@ -1348,12 +1339,12 @@
       <c r="J24" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K24" s="69"/>
-      <c r="L24" s="69"/>
-      <c r="M24" s="69"/>
-      <c r="N24" s="69"/>
-    </row>
-    <row r="25" spans="1:14" ht="20.25">
+      <c r="K24" s="68"/>
+      <c r="L24" s="68"/>
+      <c r="M24" s="68"/>
+      <c r="N24" s="68"/>
+    </row>
+    <row r="25" spans="1:14" ht="15.75">
       <c r="A25" s="36"/>
       <c r="B25" s="36"/>
       <c r="C25" s="36"/>
@@ -1366,10 +1357,10 @@
       <c r="J25" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K25" s="69"/>
-      <c r="L25" s="69"/>
-      <c r="M25" s="69"/>
-      <c r="N25" s="69"/>
+      <c r="K25" s="68"/>
+      <c r="L25" s="68"/>
+      <c r="M25" s="68"/>
+      <c r="N25" s="68"/>
     </row>
     <row r="27" spans="1:14" hidden="1"/>
     <row r="29" spans="1:14">
@@ -1384,7 +1375,7 @@
         <v>5</v>
       </c>
       <c r="K29" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L29" s="23"/>
       <c r="M29" s="23"/>
@@ -1392,7 +1383,7 @@
     <row r="30" spans="1:14" ht="17.25">
       <c r="C30" s="1"/>
       <c r="I30" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J30" s="9" t="s">
         <v>5</v>
@@ -1407,7 +1398,7 @@
       </c>
       <c r="C31" s="1"/>
       <c r="I31" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J31" s="9" t="s">
         <v>5</v>
@@ -1426,40 +1417,40 @@
       <c r="J32" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K32" s="58"/>
-      <c r="L32" s="58"/>
-      <c r="M32" s="58"/>
-      <c r="N32" s="58"/>
+      <c r="K32" s="67"/>
+      <c r="L32" s="67"/>
+      <c r="M32" s="67"/>
+      <c r="N32" s="67"/>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D33" s="12"/>
-      <c r="E33" s="57" t="s">
-        <v>52</v>
-      </c>
-      <c r="F33" s="57"/>
-      <c r="G33" s="57"/>
-      <c r="H33" s="57"/>
+      <c r="E33" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="F33" s="66"/>
+      <c r="G33" s="66"/>
+      <c r="H33" s="66"/>
       <c r="I33" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J33" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K33" s="58"/>
-      <c r="L33" s="58"/>
-      <c r="M33" s="58"/>
-      <c r="N33" s="58"/>
+      <c r="K33" s="67"/>
+      <c r="L33" s="67"/>
+      <c r="M33" s="67"/>
+      <c r="N33" s="67"/>
     </row>
     <row r="34" spans="1:15">
-      <c r="E34" s="57" t="s">
-        <v>27</v>
-      </c>
-      <c r="F34" s="57"/>
-      <c r="G34" s="57"/>
-      <c r="H34" s="57"/>
+      <c r="E34" s="66" t="s">
+        <v>26</v>
+      </c>
+      <c r="F34" s="66"/>
+      <c r="G34" s="66"/>
+      <c r="H34" s="66"/>
     </row>
     <row r="35" spans="1:15" ht="18" customHeight="1">
       <c r="D35" s="29"/>
@@ -1469,134 +1460,134 @@
       <c r="H35" s="33"/>
     </row>
     <row r="36" spans="1:15">
-      <c r="A36" s="56" t="s">
-        <v>28</v>
-      </c>
-      <c r="B36" s="56"/>
-      <c r="C36" s="50"/>
-      <c r="D36" s="50"/>
-      <c r="E36" s="50"/>
-      <c r="F36" s="50"/>
+      <c r="A36" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" s="65"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="52"/>
       <c r="G36" s="31"/>
       <c r="H36" s="31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I36" s="32"/>
       <c r="J36" s="32"/>
       <c r="K36" s="32"/>
-      <c r="L36" s="67"/>
-      <c r="M36" s="67"/>
-      <c r="N36" s="68"/>
+      <c r="L36" s="62"/>
+      <c r="M36" s="62"/>
+      <c r="N36" s="63"/>
     </row>
     <row r="37" spans="1:15" ht="3.75" customHeight="1">
       <c r="J37" s="21"/>
     </row>
     <row r="38" spans="1:15">
-      <c r="A38" s="40" t="s">
+      <c r="A38" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" s="42"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="42"/>
+      <c r="G38" s="42"/>
+      <c r="H38" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="40"/>
-      <c r="C38" s="40"/>
-      <c r="D38" s="40"/>
-      <c r="E38" s="40"/>
-      <c r="F38" s="40"/>
-      <c r="G38" s="40"/>
-      <c r="H38" s="39" t="s">
+      <c r="I38" s="40"/>
+      <c r="J38" s="40"/>
+      <c r="K38" s="40"/>
+      <c r="L38" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="I38" s="39"/>
-      <c r="J38" s="39"/>
-      <c r="K38" s="39"/>
-      <c r="L38" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="M38" s="39"/>
-      <c r="N38" s="39"/>
+      <c r="M38" s="40"/>
+      <c r="N38" s="40"/>
     </row>
     <row r="39" spans="1:15">
-      <c r="A39" s="38"/>
-      <c r="B39" s="38"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="38"/>
-      <c r="G39" s="38"/>
-      <c r="H39" s="38"/>
-      <c r="I39" s="38"/>
-      <c r="J39" s="38"/>
-      <c r="K39" s="38"/>
-      <c r="L39" s="66"/>
-      <c r="M39" s="66"/>
-      <c r="N39" s="66"/>
+      <c r="A39" s="39"/>
+      <c r="B39" s="39"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="39"/>
+      <c r="L39" s="41"/>
+      <c r="M39" s="41"/>
+      <c r="N39" s="41"/>
     </row>
     <row r="40" spans="1:15">
-      <c r="A40" s="38"/>
-      <c r="B40" s="38"/>
-      <c r="C40" s="38"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="38"/>
-      <c r="G40" s="38"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="38"/>
-      <c r="J40" s="38"/>
-      <c r="K40" s="38"/>
-      <c r="L40" s="66"/>
-      <c r="M40" s="66"/>
-      <c r="N40" s="66"/>
+      <c r="A40" s="39"/>
+      <c r="B40" s="39"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="39"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="39"/>
+      <c r="H40" s="39"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="39"/>
+      <c r="K40" s="39"/>
+      <c r="L40" s="41"/>
+      <c r="M40" s="41"/>
+      <c r="N40" s="41"/>
     </row>
     <row r="41" spans="1:15">
-      <c r="A41" s="38"/>
-      <c r="B41" s="38"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="38"/>
-      <c r="H41" s="38"/>
-      <c r="I41" s="38"/>
-      <c r="J41" s="38"/>
-      <c r="K41" s="38"/>
-      <c r="L41" s="66"/>
-      <c r="M41" s="66"/>
-      <c r="N41" s="66"/>
+      <c r="A41" s="39"/>
+      <c r="B41" s="39"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="39"/>
+      <c r="H41" s="39"/>
+      <c r="I41" s="39"/>
+      <c r="J41" s="39"/>
+      <c r="K41" s="39"/>
+      <c r="L41" s="41"/>
+      <c r="M41" s="41"/>
+      <c r="N41" s="41"/>
     </row>
     <row r="42" spans="1:15">
-      <c r="A42" s="38"/>
-      <c r="B42" s="38"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="38"/>
-      <c r="F42" s="38"/>
-      <c r="G42" s="38"/>
-      <c r="H42" s="38"/>
-      <c r="I42" s="38"/>
-      <c r="J42" s="38"/>
-      <c r="K42" s="38"/>
-      <c r="L42" s="66"/>
-      <c r="M42" s="66"/>
-      <c r="N42" s="66"/>
+      <c r="A42" s="39"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="39"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
+      <c r="K42" s="39"/>
+      <c r="L42" s="41"/>
+      <c r="M42" s="41"/>
+      <c r="N42" s="41"/>
     </row>
     <row r="43" spans="1:15" ht="3.75" customHeight="1"/>
     <row r="44" spans="1:15">
-      <c r="A44" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="B44" s="46"/>
-      <c r="C44" s="71"/>
-      <c r="D44" s="71"/>
-      <c r="E44" s="71"/>
-      <c r="F44" s="71"/>
-      <c r="G44" s="71"/>
-      <c r="H44" s="71"/>
-      <c r="I44" s="72"/>
+      <c r="A44" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" s="48"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="54"/>
       <c r="J44" s="14"/>
       <c r="K44" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="L44" s="52"/>
-      <c r="M44" s="52"/>
-      <c r="N44" s="53"/>
+        <v>48</v>
+      </c>
+      <c r="L44" s="60"/>
+      <c r="M44" s="60"/>
+      <c r="N44" s="61"/>
     </row>
     <row r="45" spans="1:15" ht="8.25" customHeight="1">
       <c r="A45" s="16"/>
@@ -1616,217 +1607,217 @@
     </row>
     <row r="46" spans="1:15" ht="3" customHeight="1"/>
     <row r="47" spans="1:15">
-      <c r="A47" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="B47" s="48"/>
-      <c r="C47" s="48"/>
-      <c r="D47" s="48"/>
-      <c r="E47" s="48"/>
-      <c r="F47" s="48"/>
-      <c r="G47" s="48"/>
-      <c r="H47" s="48"/>
-      <c r="I47" s="49"/>
+      <c r="A47" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" s="50"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="50"/>
+      <c r="H47" s="50"/>
+      <c r="I47" s="51"/>
     </row>
     <row r="48" spans="1:15">
-      <c r="A48" s="41" t="s">
-        <v>34</v>
-      </c>
-      <c r="B48" s="42"/>
+      <c r="A48" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" s="44"/>
       <c r="C48" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D48" s="62"/>
-      <c r="E48" s="62"/>
-      <c r="F48" s="62"/>
-      <c r="G48" s="62"/>
-      <c r="H48" s="62"/>
-      <c r="I48" s="63"/>
-      <c r="K48" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="L48" s="51"/>
-      <c r="M48" s="51"/>
-      <c r="N48" s="51"/>
+      <c r="D48" s="55"/>
+      <c r="E48" s="55"/>
+      <c r="F48" s="55"/>
+      <c r="G48" s="55"/>
+      <c r="H48" s="55"/>
+      <c r="I48" s="56"/>
+      <c r="K48" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="L48" s="59"/>
+      <c r="M48" s="59"/>
+      <c r="N48" s="59"/>
       <c r="O48" s="11"/>
     </row>
     <row r="49" spans="1:14">
-      <c r="A49" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="B49" s="42"/>
+      <c r="A49" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="B49" s="44"/>
       <c r="C49" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D49" s="62"/>
-      <c r="E49" s="62"/>
-      <c r="F49" s="62"/>
-      <c r="G49" s="62"/>
-      <c r="H49" s="62"/>
-      <c r="I49" s="63"/>
+      <c r="D49" s="55"/>
+      <c r="E49" s="55"/>
+      <c r="F49" s="55"/>
+      <c r="G49" s="55"/>
+      <c r="H49" s="55"/>
+      <c r="I49" s="56"/>
       <c r="J49" s="11"/>
-      <c r="K49" s="51"/>
-      <c r="L49" s="51"/>
-      <c r="M49" s="51"/>
-      <c r="N49" s="51"/>
+      <c r="K49" s="59"/>
+      <c r="L49" s="59"/>
+      <c r="M49" s="59"/>
+      <c r="N49" s="59"/>
     </row>
     <row r="50" spans="1:14" ht="15" customHeight="1">
-      <c r="A50" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="B50" s="44"/>
+      <c r="A50" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" s="46"/>
       <c r="C50" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D50" s="64"/>
-      <c r="E50" s="64"/>
-      <c r="F50" s="64"/>
-      <c r="G50" s="64"/>
-      <c r="H50" s="64"/>
-      <c r="I50" s="65"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="57"/>
+      <c r="F50" s="57"/>
+      <c r="G50" s="57"/>
+      <c r="H50" s="57"/>
+      <c r="I50" s="58"/>
     </row>
     <row r="51" spans="1:14" ht="4.5" customHeight="1"/>
     <row r="52" spans="1:14">
-      <c r="A52" s="50" t="s">
+      <c r="A52" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="B52" s="52"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="E52" s="52"/>
+      <c r="F52" s="52"/>
+      <c r="G52" s="52"/>
+      <c r="H52" s="52"/>
+      <c r="I52" s="52"/>
+      <c r="J52" s="10"/>
+      <c r="K52" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="L52" s="52"/>
+      <c r="M52" s="52"/>
+      <c r="N52" s="52"/>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="A53" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="B52" s="50"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="50" t="s">
+      <c r="B53" s="52"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="E53" s="52"/>
+      <c r="F53" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="G53" s="52"/>
+      <c r="H53" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="I53" s="52"/>
+      <c r="J53" s="28"/>
+      <c r="K53" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="L53" s="52"/>
+      <c r="M53" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="N53" s="52"/>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" s="52"/>
+      <c r="B54" s="52"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="52"/>
+      <c r="E54" s="52"/>
+      <c r="F54" s="52"/>
+      <c r="G54" s="52"/>
+      <c r="H54" s="52"/>
+      <c r="I54" s="52"/>
+      <c r="J54" s="10"/>
+      <c r="K54" s="52"/>
+      <c r="L54" s="52"/>
+      <c r="M54" s="52"/>
+      <c r="N54" s="52"/>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="A55" s="52"/>
+      <c r="B55" s="52"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="52"/>
+      <c r="E55" s="52"/>
+      <c r="F55" s="52"/>
+      <c r="G55" s="52"/>
+      <c r="H55" s="52"/>
+      <c r="I55" s="52"/>
+      <c r="J55" s="10"/>
+      <c r="K55" s="52"/>
+      <c r="L55" s="52"/>
+      <c r="M55" s="52"/>
+      <c r="N55" s="52"/>
+    </row>
+    <row r="56" spans="1:14">
+      <c r="A56" s="52"/>
+      <c r="B56" s="52"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="52"/>
+      <c r="E56" s="52"/>
+      <c r="F56" s="52"/>
+      <c r="G56" s="52"/>
+      <c r="H56" s="52"/>
+      <c r="I56" s="52"/>
+      <c r="J56" s="10"/>
+      <c r="K56" s="52"/>
+      <c r="L56" s="52"/>
+      <c r="M56" s="52"/>
+      <c r="N56" s="52"/>
+    </row>
+    <row r="57" spans="1:14">
+      <c r="A57" s="52"/>
+      <c r="B57" s="52"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="52"/>
+      <c r="E57" s="52"/>
+      <c r="F57" s="52"/>
+      <c r="G57" s="52"/>
+      <c r="H57" s="52"/>
+      <c r="I57" s="52"/>
+      <c r="J57" s="10"/>
+      <c r="K57" s="52"/>
+      <c r="L57" s="52"/>
+      <c r="M57" s="52"/>
+      <c r="N57" s="52"/>
+    </row>
+    <row r="58" spans="1:14">
+      <c r="A58" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="B58" s="52"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="E58" s="52"/>
+      <c r="F58" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="E52" s="50"/>
-      <c r="F52" s="50"/>
-      <c r="G52" s="50"/>
-      <c r="H52" s="50"/>
-      <c r="I52" s="50"/>
-      <c r="J52" s="10"/>
-      <c r="K52" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="L52" s="50"/>
-      <c r="M52" s="50"/>
-      <c r="N52" s="50"/>
-    </row>
-    <row r="53" spans="1:14">
-      <c r="A53" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="B53" s="50"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="E53" s="50"/>
-      <c r="F53" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="G53" s="50"/>
-      <c r="H53" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="I53" s="50"/>
-      <c r="J53" s="28"/>
-      <c r="K53" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="L53" s="50"/>
-      <c r="M53" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="N53" s="50"/>
-    </row>
-    <row r="54" spans="1:14">
-      <c r="A54" s="50"/>
-      <c r="B54" s="50"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="50"/>
-      <c r="E54" s="50"/>
-      <c r="F54" s="50"/>
-      <c r="G54" s="50"/>
-      <c r="H54" s="50"/>
-      <c r="I54" s="50"/>
-      <c r="J54" s="10"/>
-      <c r="K54" s="50"/>
-      <c r="L54" s="50"/>
-      <c r="M54" s="50"/>
-      <c r="N54" s="50"/>
-    </row>
-    <row r="55" spans="1:14">
-      <c r="A55" s="50"/>
-      <c r="B55" s="50"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="50"/>
-      <c r="E55" s="50"/>
-      <c r="F55" s="50"/>
-      <c r="G55" s="50"/>
-      <c r="H55" s="50"/>
-      <c r="I55" s="50"/>
-      <c r="J55" s="10"/>
-      <c r="K55" s="50"/>
-      <c r="L55" s="50"/>
-      <c r="M55" s="50"/>
-      <c r="N55" s="50"/>
-    </row>
-    <row r="56" spans="1:14">
-      <c r="A56" s="50"/>
-      <c r="B56" s="50"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="50"/>
-      <c r="E56" s="50"/>
-      <c r="F56" s="50"/>
-      <c r="G56" s="50"/>
-      <c r="H56" s="50"/>
-      <c r="I56" s="50"/>
-      <c r="J56" s="10"/>
-      <c r="K56" s="50"/>
-      <c r="L56" s="50"/>
-      <c r="M56" s="50"/>
-      <c r="N56" s="50"/>
-    </row>
-    <row r="57" spans="1:14">
-      <c r="A57" s="50"/>
-      <c r="B57" s="50"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="50"/>
-      <c r="E57" s="50"/>
-      <c r="F57" s="50"/>
-      <c r="G57" s="50"/>
-      <c r="H57" s="50"/>
-      <c r="I57" s="50"/>
-      <c r="J57" s="10"/>
-      <c r="K57" s="50"/>
-      <c r="L57" s="50"/>
-      <c r="M57" s="50"/>
-      <c r="N57" s="50"/>
-    </row>
-    <row r="58" spans="1:14">
-      <c r="A58" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="B58" s="50"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="E58" s="50"/>
-      <c r="F58" s="50" t="s">
+      <c r="G58" s="52"/>
+      <c r="H58" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="G58" s="50"/>
-      <c r="H58" s="50" t="s">
+      <c r="I58" s="52"/>
+      <c r="J58" s="10"/>
+      <c r="K58" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="I58" s="50"/>
-      <c r="J58" s="10"/>
-      <c r="K58" s="50" t="s">
+      <c r="L58" s="52"/>
+      <c r="M58" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="L58" s="50"/>
-      <c r="M58" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="N58" s="50"/>
+      <c r="N58" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="83">

</xml_diff>

<commit_message>
dev-3.0 : print setalah submit, terbilang mata uang asing
</commit_message>
<xml_diff>
--- a/storage/template/tandaterima.xlsx
+++ b/storage/template/tandaterima.xlsx
@@ -198,7 +198,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,6 +275,12 @@
       <name val="Free 3 of 9"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -428,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -473,102 +479,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -581,20 +491,137 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -971,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L46" sqref="L46:N46"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38:H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -998,12 +1025,12 @@
       <c r="J5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="28" t="s">
+      <c r="K5" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
       <c r="O5" s="27"/>
     </row>
     <row r="6" spans="1:15" ht="15.75">
@@ -1013,32 +1040,32 @@
       <c r="J6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="67"/>
+      <c r="N6" s="67"/>
     </row>
     <row r="7" spans="1:15" ht="17.25">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
+      <c r="L7" s="69"/>
+      <c r="M7" s="69"/>
+      <c r="N7" s="69"/>
     </row>
     <row r="8" spans="1:15" ht="17.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="69"/>
+      <c r="K8" s="69"/>
+      <c r="L8" s="69"/>
+      <c r="M8" s="69"/>
+      <c r="N8" s="69"/>
     </row>
     <row r="9" spans="1:15" ht="17.25">
       <c r="A9" s="1" t="s">
@@ -1050,10 +1077,10 @@
       <c r="J9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="49"/>
+      <c r="N9" s="49"/>
     </row>
     <row r="10" spans="1:15" ht="16.5" customHeight="1">
       <c r="F10" s="5" t="s">
@@ -1061,39 +1088,39 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="17.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="28"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="68"/>
+      <c r="K11" s="68"/>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:15" ht="17.25">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="28"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="68"/>
+      <c r="K12" s="68"/>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1">
@@ -1114,196 +1141,202 @@
       <c r="A14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40" t="s">
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40" t="s">
+      <c r="G14" s="61"/>
+      <c r="H14" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="40"/>
-      <c r="L14" s="40" t="s">
+      <c r="I14" s="61"/>
+      <c r="J14" s="61"/>
+      <c r="K14" s="61"/>
+      <c r="L14" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="M14" s="40"/>
-      <c r="N14" s="40"/>
+      <c r="M14" s="61"/>
+      <c r="N14" s="61"/>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="32">
+      <c r="A15" s="48">
         <v>1</v>
       </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="32"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="48"/>
+      <c r="K15" s="48"/>
+      <c r="L15" s="48"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="48"/>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="32"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="32"/>
+      <c r="A16" s="48"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="48"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="48"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="32"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="32"/>
+      <c r="A17" s="48"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="48"/>
     </row>
     <row r="18" spans="1:14" ht="17.25">
       <c r="A18" s="6"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="41"/>
-      <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="32"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="52"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="48"/>
     </row>
     <row r="19" spans="1:14" ht="6.75" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
+      <c r="D19" s="77"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="77"/>
+      <c r="G19" s="77"/>
+      <c r="H19" s="77"/>
+      <c r="I19" s="77"/>
+      <c r="J19" s="77"/>
+      <c r="K19" s="77"/>
+      <c r="L19" s="77"/>
+      <c r="M19" s="77"/>
+      <c r="N19" s="77"/>
     </row>
     <row r="20" spans="1:14" ht="15.75">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="28"/>
+      <c r="B20" s="49"/>
       <c r="C20" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="35"/>
-      <c r="L20" s="35"/>
-      <c r="M20" s="35"/>
-      <c r="N20" s="35"/>
+      <c r="D20" s="78"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="78"/>
+      <c r="G20" s="78"/>
+      <c r="H20" s="78"/>
+      <c r="I20" s="78"/>
+      <c r="J20" s="78"/>
+      <c r="K20" s="78"/>
+      <c r="L20" s="78"/>
+      <c r="M20" s="78"/>
+      <c r="N20" s="78"/>
     </row>
     <row r="21" spans="1:14" ht="6.75" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
+      <c r="D21" s="78"/>
+      <c r="E21" s="78"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="78"/>
+      <c r="H21" s="78"/>
+      <c r="I21" s="78"/>
+      <c r="J21" s="78"/>
+      <c r="K21" s="78"/>
+      <c r="L21" s="78"/>
+      <c r="M21" s="78"/>
+      <c r="N21" s="78"/>
     </row>
     <row r="22" spans="1:14" ht="17.25">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="42"/>
-      <c r="C22" s="42" t="s">
+      <c r="B22" s="51"/>
+      <c r="C22" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
       <c r="F22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="7" t="s">
         <v>17</v>
       </c>
       <c r="J22" s="1"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="36"/>
-      <c r="N22" s="36"/>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23" s="43"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-    </row>
-    <row r="24" spans="1:14" ht="15.75">
-      <c r="A24" s="43"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="G24" s="7" t="s">
+      <c r="K22" s="66"/>
+      <c r="L22" s="66"/>
+      <c r="M22" s="66"/>
+      <c r="N22" s="66"/>
+    </row>
+    <row r="23" spans="1:14" ht="15.75">
+      <c r="A23" s="50"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="G23" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7" t="s">
+      <c r="I23" s="7"/>
+      <c r="J23" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K24" s="35"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="35"/>
-      <c r="N24" s="35"/>
+      <c r="K23" s="72"/>
+      <c r="L23" s="72"/>
+      <c r="M23" s="72"/>
+      <c r="N23" s="72"/>
+    </row>
+    <row r="24" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A24" s="50"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="K24" s="72"/>
+      <c r="L24" s="72"/>
+      <c r="M24" s="72"/>
+      <c r="N24" s="72"/>
     </row>
     <row r="25" spans="1:14" ht="15.75">
-      <c r="A25" s="43"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
       <c r="G25" s="7" t="s">
         <v>19</v>
       </c>
@@ -1311,17 +1344,17 @@
       <c r="J25" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K25" s="35"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="35"/>
-      <c r="N25" s="35"/>
+      <c r="K25" s="65"/>
+      <c r="L25" s="65"/>
+      <c r="M25" s="65"/>
+      <c r="N25" s="65"/>
     </row>
     <row r="26" spans="1:14" ht="15.75">
-      <c r="A26" s="43"/>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
+      <c r="A26" s="50"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
       <c r="G26" s="7" t="s">
         <v>20</v>
       </c>
@@ -1329,17 +1362,17 @@
       <c r="J26" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K26" s="35"/>
-      <c r="L26" s="35"/>
-      <c r="M26" s="35"/>
-      <c r="N26" s="35"/>
+      <c r="K26" s="65"/>
+      <c r="L26" s="65"/>
+      <c r="M26" s="65"/>
+      <c r="N26" s="65"/>
     </row>
     <row r="27" spans="1:14" ht="15.75">
-      <c r="A27" s="43"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
+      <c r="A27" s="50"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
       <c r="G27" s="7" t="s">
         <v>21</v>
       </c>
@@ -1347,10 +1380,10 @@
       <c r="J27" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K27" s="35"/>
-      <c r="L27" s="35"/>
-      <c r="M27" s="35"/>
-      <c r="N27" s="35"/>
+      <c r="K27" s="65"/>
+      <c r="L27" s="65"/>
+      <c r="M27" s="65"/>
+      <c r="N27" s="65"/>
     </row>
     <row r="29" spans="1:14" ht="40.5" customHeight="1"/>
     <row r="31" spans="1:14">
@@ -1407,436 +1440,451 @@
       <c r="J34" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K34" s="34"/>
-      <c r="L34" s="34"/>
-      <c r="M34" s="34"/>
-      <c r="N34" s="34"/>
+      <c r="K34" s="64"/>
+      <c r="L34" s="64"/>
+      <c r="M34" s="64"/>
+      <c r="N34" s="64"/>
     </row>
     <row r="35" spans="1:14">
       <c r="A35" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D35" s="12"/>
-      <c r="E35" s="33" t="s">
+      <c r="E35" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="F35" s="33"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="33"/>
+      <c r="F35" s="63"/>
+      <c r="G35" s="63"/>
+      <c r="H35" s="63"/>
       <c r="I35" s="9" t="s">
         <v>25</v>
       </c>
       <c r="J35" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K35" s="34"/>
-      <c r="L35" s="34"/>
-      <c r="M35" s="34"/>
-      <c r="N35" s="34"/>
+      <c r="K35" s="64"/>
+      <c r="L35" s="64"/>
+      <c r="M35" s="64"/>
+      <c r="N35" s="64"/>
     </row>
     <row r="36" spans="1:14">
-      <c r="E36" s="33" t="s">
+      <c r="E36" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="F36" s="33"/>
-      <c r="G36" s="33"/>
-      <c r="H36" s="33"/>
+      <c r="F36" s="63"/>
+      <c r="G36" s="63"/>
+      <c r="H36" s="63"/>
     </row>
     <row r="37" spans="1:14" ht="18" customHeight="1">
       <c r="D37" s="26"/>
-      <c r="E37" s="57"/>
-      <c r="F37" s="57"/>
-      <c r="G37" s="57"/>
-      <c r="H37" s="57"/>
+      <c r="E37" s="47"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="47"/>
+      <c r="H37" s="47"/>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="44" t="s">
+      <c r="A38" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="44"/>
-      <c r="C38" s="45"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="45"/>
-      <c r="F38" s="45"/>
-      <c r="G38" s="46"/>
-      <c r="H38" s="46" t="s">
+      <c r="B38" s="62"/>
+      <c r="C38" s="79"/>
+      <c r="D38" s="80"/>
+      <c r="E38" s="80"/>
+      <c r="F38" s="80"/>
+      <c r="G38" s="80"/>
+      <c r="H38" s="81"/>
+      <c r="I38" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="I38" s="39"/>
-      <c r="J38" s="39"/>
-      <c r="K38" s="39"/>
-      <c r="L38" s="37"/>
-      <c r="M38" s="37"/>
-      <c r="N38" s="38"/>
+      <c r="J38" s="46"/>
+      <c r="K38" s="46"/>
+      <c r="L38" s="59"/>
+      <c r="M38" s="59"/>
+      <c r="N38" s="60"/>
     </row>
     <row r="39" spans="1:14" ht="3.75" customHeight="1">
       <c r="J39" s="19"/>
     </row>
     <row r="40" spans="1:14">
-      <c r="A40" s="56" t="s">
+      <c r="A40" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="56"/>
-      <c r="C40" s="56"/>
-      <c r="D40" s="56"/>
-      <c r="E40" s="56"/>
-      <c r="F40" s="56"/>
-      <c r="G40" s="56"/>
-      <c r="H40" s="56" t="s">
+      <c r="B40" s="53"/>
+      <c r="C40" s="53"/>
+      <c r="D40" s="53"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="I40" s="56"/>
-      <c r="J40" s="56"/>
-      <c r="K40" s="56"/>
-      <c r="L40" s="56" t="s">
+      <c r="I40" s="53"/>
+      <c r="J40" s="53"/>
+      <c r="K40" s="53"/>
+      <c r="L40" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="M40" s="56"/>
-      <c r="N40" s="56"/>
+      <c r="M40" s="53"/>
+      <c r="N40" s="53"/>
     </row>
     <row r="41" spans="1:14">
-      <c r="A41" s="54"/>
-      <c r="B41" s="54"/>
-      <c r="C41" s="54"/>
-      <c r="D41" s="54"/>
-      <c r="E41" s="54"/>
-      <c r="F41" s="54"/>
-      <c r="G41" s="54"/>
-      <c r="H41" s="54"/>
-      <c r="I41" s="54"/>
-      <c r="J41" s="54"/>
-      <c r="K41" s="54"/>
-      <c r="L41" s="55"/>
-      <c r="M41" s="55"/>
-      <c r="N41" s="55"/>
+      <c r="A41" s="70"/>
+      <c r="B41" s="70"/>
+      <c r="C41" s="70"/>
+      <c r="D41" s="70"/>
+      <c r="E41" s="70"/>
+      <c r="F41" s="70"/>
+      <c r="G41" s="70"/>
+      <c r="H41" s="70"/>
+      <c r="I41" s="70"/>
+      <c r="J41" s="70"/>
+      <c r="K41" s="70"/>
+      <c r="L41" s="71"/>
+      <c r="M41" s="71"/>
+      <c r="N41" s="71"/>
     </row>
     <row r="42" spans="1:14">
-      <c r="A42" s="54"/>
-      <c r="B42" s="54"/>
-      <c r="C42" s="54"/>
-      <c r="D42" s="54"/>
-      <c r="E42" s="54"/>
-      <c r="F42" s="54"/>
-      <c r="G42" s="54"/>
-      <c r="H42" s="54"/>
-      <c r="I42" s="54"/>
-      <c r="J42" s="54"/>
-      <c r="K42" s="54"/>
-      <c r="L42" s="55"/>
-      <c r="M42" s="55"/>
-      <c r="N42" s="55"/>
+      <c r="A42" s="70"/>
+      <c r="B42" s="70"/>
+      <c r="C42" s="70"/>
+      <c r="D42" s="70"/>
+      <c r="E42" s="70"/>
+      <c r="F42" s="70"/>
+      <c r="G42" s="70"/>
+      <c r="H42" s="70"/>
+      <c r="I42" s="70"/>
+      <c r="J42" s="70"/>
+      <c r="K42" s="70"/>
+      <c r="L42" s="71"/>
+      <c r="M42" s="71"/>
+      <c r="N42" s="71"/>
     </row>
     <row r="43" spans="1:14">
-      <c r="A43" s="54"/>
-      <c r="B43" s="54"/>
-      <c r="C43" s="54"/>
-      <c r="D43" s="54"/>
-      <c r="E43" s="54"/>
-      <c r="F43" s="54"/>
-      <c r="G43" s="54"/>
-      <c r="H43" s="54"/>
-      <c r="I43" s="54"/>
-      <c r="J43" s="54"/>
-      <c r="K43" s="54"/>
-      <c r="L43" s="55"/>
-      <c r="M43" s="55"/>
-      <c r="N43" s="55"/>
+      <c r="A43" s="70"/>
+      <c r="B43" s="70"/>
+      <c r="C43" s="70"/>
+      <c r="D43" s="70"/>
+      <c r="E43" s="70"/>
+      <c r="F43" s="70"/>
+      <c r="G43" s="70"/>
+      <c r="H43" s="70"/>
+      <c r="I43" s="70"/>
+      <c r="J43" s="70"/>
+      <c r="K43" s="70"/>
+      <c r="L43" s="71"/>
+      <c r="M43" s="71"/>
+      <c r="N43" s="71"/>
     </row>
     <row r="44" spans="1:14">
-      <c r="A44" s="54"/>
-      <c r="B44" s="54"/>
-      <c r="C44" s="54"/>
-      <c r="D44" s="54"/>
-      <c r="E44" s="54"/>
-      <c r="F44" s="54"/>
-      <c r="G44" s="54"/>
-      <c r="H44" s="54"/>
-      <c r="I44" s="54"/>
-      <c r="J44" s="54"/>
-      <c r="K44" s="54"/>
-      <c r="L44" s="55"/>
-      <c r="M44" s="55"/>
-      <c r="N44" s="55"/>
+      <c r="A44" s="70"/>
+      <c r="B44" s="70"/>
+      <c r="C44" s="70"/>
+      <c r="D44" s="70"/>
+      <c r="E44" s="70"/>
+      <c r="F44" s="70"/>
+      <c r="G44" s="70"/>
+      <c r="H44" s="70"/>
+      <c r="I44" s="70"/>
+      <c r="J44" s="70"/>
+      <c r="K44" s="70"/>
+      <c r="L44" s="71"/>
+      <c r="M44" s="71"/>
+      <c r="N44" s="71"/>
     </row>
     <row r="45" spans="1:14" ht="3.75" customHeight="1"/>
     <row r="46" spans="1:14">
-      <c r="A46" s="52" t="s">
+      <c r="A46" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="53"/>
-      <c r="C46" s="72"/>
-      <c r="D46" s="72"/>
-      <c r="E46" s="72"/>
-      <c r="F46" s="72"/>
-      <c r="G46" s="72"/>
-      <c r="H46" s="72"/>
-      <c r="I46" s="72"/>
-      <c r="J46" s="72"/>
-      <c r="K46" s="73"/>
-      <c r="L46" s="74"/>
-      <c r="M46" s="58"/>
-      <c r="N46" s="59"/>
-    </row>
-    <row r="47" spans="1:14" ht="8.25" customHeight="1">
+      <c r="B46" s="55"/>
+      <c r="C46" s="73"/>
+      <c r="D46" s="73"/>
+      <c r="E46" s="73"/>
+      <c r="F46" s="73"/>
+      <c r="G46" s="73"/>
+      <c r="H46" s="73"/>
+      <c r="I46" s="73"/>
+      <c r="J46" s="73"/>
+      <c r="K46" s="74"/>
+      <c r="L46" s="38"/>
+      <c r="M46" s="39"/>
+      <c r="N46" s="40"/>
+    </row>
+    <row r="47" spans="1:14" ht="15" customHeight="1">
       <c r="A47" s="14"/>
       <c r="B47" s="15"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15"/>
-      <c r="H47" s="15"/>
-      <c r="I47" s="15"/>
-      <c r="J47" s="15"/>
-      <c r="K47" s="16"/>
+      <c r="C47" s="75"/>
+      <c r="D47" s="75"/>
+      <c r="E47" s="75"/>
+      <c r="F47" s="75"/>
+      <c r="G47" s="75"/>
+      <c r="H47" s="75"/>
+      <c r="I47" s="75"/>
+      <c r="J47" s="75"/>
+      <c r="K47" s="76"/>
       <c r="L47" s="14"/>
       <c r="M47" s="15"/>
       <c r="N47" s="16"/>
     </row>
-    <row r="48" spans="1:14" ht="3" customHeight="1"/>
+    <row r="48" spans="1:14" ht="9" customHeight="1"/>
     <row r="49" spans="1:15">
-      <c r="A49" s="60" t="s">
+      <c r="A49" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B49" s="60"/>
-      <c r="C49" s="61"/>
-      <c r="D49" s="61"/>
-      <c r="E49" s="61"/>
-      <c r="F49" s="61"/>
-      <c r="G49" s="61"/>
-      <c r="H49" s="61"/>
-      <c r="I49" s="61"/>
-      <c r="J49" s="64"/>
-      <c r="K49" s="65"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="29"/>
+      <c r="J49" s="32"/>
+      <c r="K49" s="33"/>
     </row>
     <row r="50" spans="1:15">
-      <c r="A50" s="62" t="s">
+      <c r="A50" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B50" s="66"/>
-      <c r="C50" s="67" t="s">
+      <c r="B50" s="34"/>
+      <c r="C50" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D50" s="70"/>
-      <c r="E50" s="70"/>
-      <c r="F50" s="70"/>
-      <c r="G50" s="70"/>
-      <c r="H50" s="70"/>
-      <c r="I50" s="70"/>
-      <c r="J50" s="70"/>
-      <c r="K50" s="71"/>
-      <c r="L50" s="51" t="s">
+      <c r="D50" s="42"/>
+      <c r="E50" s="42"/>
+      <c r="F50" s="42"/>
+      <c r="G50" s="42"/>
+      <c r="H50" s="42"/>
+      <c r="I50" s="42"/>
+      <c r="J50" s="42"/>
+      <c r="K50" s="43"/>
+      <c r="L50" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="M50" s="51"/>
-      <c r="N50" s="51"/>
+      <c r="M50" s="41"/>
+      <c r="N50" s="41"/>
       <c r="O50" s="11"/>
     </row>
     <row r="51" spans="1:15">
-      <c r="A51" s="62" t="s">
+      <c r="A51" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B51" s="68"/>
+      <c r="B51" s="36"/>
       <c r="C51" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D51" s="47"/>
-      <c r="E51" s="47"/>
-      <c r="F51" s="47"/>
-      <c r="G51" s="47"/>
-      <c r="H51" s="47"/>
-      <c r="I51" s="47"/>
-      <c r="J51" s="47"/>
-      <c r="K51" s="48"/>
-      <c r="L51" s="51"/>
-      <c r="M51" s="51"/>
-      <c r="N51" s="51"/>
+      <c r="D51" s="44"/>
+      <c r="E51" s="44"/>
+      <c r="F51" s="44"/>
+      <c r="G51" s="44"/>
+      <c r="H51" s="44"/>
+      <c r="I51" s="44"/>
+      <c r="J51" s="44"/>
+      <c r="K51" s="45"/>
+      <c r="L51" s="41"/>
+      <c r="M51" s="41"/>
+      <c r="N51" s="41"/>
     </row>
     <row r="52" spans="1:15" ht="15" customHeight="1">
-      <c r="A52" s="63" t="s">
+      <c r="A52" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="69"/>
+      <c r="B52" s="37"/>
       <c r="C52" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D52" s="49"/>
-      <c r="E52" s="49"/>
-      <c r="F52" s="49"/>
-      <c r="G52" s="49"/>
-      <c r="H52" s="49"/>
-      <c r="I52" s="49"/>
-      <c r="J52" s="49"/>
-      <c r="K52" s="50"/>
+      <c r="D52" s="56"/>
+      <c r="E52" s="56"/>
+      <c r="F52" s="56"/>
+      <c r="G52" s="56"/>
+      <c r="H52" s="56"/>
+      <c r="I52" s="56"/>
+      <c r="J52" s="56"/>
+      <c r="K52" s="57"/>
     </row>
     <row r="53" spans="1:15" ht="4.5" customHeight="1"/>
     <row r="54" spans="1:15">
-      <c r="A54" s="45" t="s">
+      <c r="A54" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="B54" s="45"/>
+      <c r="B54" s="58"/>
       <c r="C54" s="10"/>
-      <c r="D54" s="45" t="s">
+      <c r="D54" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="E54" s="45"/>
-      <c r="F54" s="45"/>
-      <c r="G54" s="45"/>
-      <c r="H54" s="45"/>
-      <c r="I54" s="45"/>
+      <c r="E54" s="58"/>
+      <c r="F54" s="58"/>
+      <c r="G54" s="58"/>
+      <c r="H54" s="58"/>
+      <c r="I54" s="58"/>
       <c r="J54" s="10"/>
-      <c r="K54" s="45" t="s">
+      <c r="K54" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="L54" s="45"/>
-      <c r="M54" s="45"/>
-      <c r="N54" s="45"/>
+      <c r="L54" s="58"/>
+      <c r="M54" s="58"/>
+      <c r="N54" s="58"/>
     </row>
     <row r="55" spans="1:15">
-      <c r="A55" s="45" t="s">
+      <c r="A55" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="B55" s="45"/>
+      <c r="B55" s="58"/>
       <c r="C55" s="10"/>
-      <c r="D55" s="45" t="s">
+      <c r="D55" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="E55" s="45"/>
-      <c r="F55" s="45" t="s">
+      <c r="E55" s="58"/>
+      <c r="F55" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="G55" s="45"/>
-      <c r="H55" s="45" t="s">
+      <c r="G55" s="58"/>
+      <c r="H55" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="I55" s="45"/>
+      <c r="I55" s="58"/>
       <c r="J55" s="25"/>
-      <c r="K55" s="45" t="s">
+      <c r="K55" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="L55" s="45"/>
-      <c r="M55" s="45" t="s">
+      <c r="L55" s="58"/>
+      <c r="M55" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="N55" s="45"/>
+      <c r="N55" s="58"/>
     </row>
     <row r="56" spans="1:15">
-      <c r="A56" s="45"/>
-      <c r="B56" s="45"/>
+      <c r="A56" s="58"/>
+      <c r="B56" s="58"/>
       <c r="C56" s="10"/>
-      <c r="D56" s="45"/>
-      <c r="E56" s="45"/>
-      <c r="F56" s="45"/>
-      <c r="G56" s="45"/>
-      <c r="H56" s="45"/>
-      <c r="I56" s="45"/>
+      <c r="D56" s="58"/>
+      <c r="E56" s="58"/>
+      <c r="F56" s="58"/>
+      <c r="G56" s="58"/>
+      <c r="H56" s="58"/>
+      <c r="I56" s="58"/>
       <c r="J56" s="10"/>
-      <c r="K56" s="45"/>
-      <c r="L56" s="45"/>
-      <c r="M56" s="45"/>
-      <c r="N56" s="45"/>
+      <c r="K56" s="58"/>
+      <c r="L56" s="58"/>
+      <c r="M56" s="58"/>
+      <c r="N56" s="58"/>
     </row>
     <row r="57" spans="1:15">
-      <c r="A57" s="45"/>
-      <c r="B57" s="45"/>
+      <c r="A57" s="58"/>
+      <c r="B57" s="58"/>
       <c r="C57" s="10"/>
-      <c r="D57" s="45"/>
-      <c r="E57" s="45"/>
-      <c r="F57" s="45"/>
-      <c r="G57" s="45"/>
-      <c r="H57" s="45"/>
-      <c r="I57" s="45"/>
+      <c r="D57" s="58"/>
+      <c r="E57" s="58"/>
+      <c r="F57" s="58"/>
+      <c r="G57" s="58"/>
+      <c r="H57" s="58"/>
+      <c r="I57" s="58"/>
       <c r="J57" s="10"/>
-      <c r="K57" s="45"/>
-      <c r="L57" s="45"/>
-      <c r="M57" s="45"/>
-      <c r="N57" s="45"/>
+      <c r="K57" s="58"/>
+      <c r="L57" s="58"/>
+      <c r="M57" s="58"/>
+      <c r="N57" s="58"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="45"/>
-      <c r="B58" s="45"/>
+      <c r="A58" s="58"/>
+      <c r="B58" s="58"/>
       <c r="C58" s="10"/>
-      <c r="D58" s="45"/>
-      <c r="E58" s="45"/>
-      <c r="F58" s="45"/>
-      <c r="G58" s="45"/>
-      <c r="H58" s="45"/>
-      <c r="I58" s="45"/>
+      <c r="D58" s="58"/>
+      <c r="E58" s="58"/>
+      <c r="F58" s="58"/>
+      <c r="G58" s="58"/>
+      <c r="H58" s="58"/>
+      <c r="I58" s="58"/>
       <c r="J58" s="10"/>
-      <c r="K58" s="45"/>
-      <c r="L58" s="45"/>
-      <c r="M58" s="45"/>
-      <c r="N58" s="45"/>
+      <c r="K58" s="58"/>
+      <c r="L58" s="58"/>
+      <c r="M58" s="58"/>
+      <c r="N58" s="58"/>
     </row>
     <row r="59" spans="1:15">
-      <c r="A59" s="45"/>
-      <c r="B59" s="45"/>
+      <c r="A59" s="58"/>
+      <c r="B59" s="58"/>
       <c r="C59" s="10"/>
-      <c r="D59" s="45"/>
-      <c r="E59" s="45"/>
-      <c r="F59" s="45"/>
-      <c r="G59" s="45"/>
-      <c r="H59" s="45"/>
-      <c r="I59" s="45"/>
+      <c r="D59" s="58"/>
+      <c r="E59" s="58"/>
+      <c r="F59" s="58"/>
+      <c r="G59" s="58"/>
+      <c r="H59" s="58"/>
+      <c r="I59" s="58"/>
       <c r="J59" s="10"/>
-      <c r="K59" s="45"/>
-      <c r="L59" s="45"/>
-      <c r="M59" s="45"/>
-      <c r="N59" s="45"/>
+      <c r="K59" s="58"/>
+      <c r="L59" s="58"/>
+      <c r="M59" s="58"/>
+      <c r="N59" s="58"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="45" t="s">
+      <c r="A60" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="45"/>
+      <c r="B60" s="58"/>
       <c r="C60" s="10"/>
-      <c r="D60" s="45" t="s">
+      <c r="D60" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="E60" s="45"/>
-      <c r="F60" s="45" t="s">
+      <c r="E60" s="58"/>
+      <c r="F60" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="G60" s="45"/>
-      <c r="H60" s="45" t="s">
+      <c r="G60" s="58"/>
+      <c r="H60" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="I60" s="45"/>
+      <c r="I60" s="58"/>
       <c r="J60" s="10"/>
-      <c r="K60" s="45" t="s">
+      <c r="K60" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="L60" s="45"/>
-      <c r="M60" s="45" t="s">
+      <c r="L60" s="58"/>
+      <c r="M60" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="N60" s="45"/>
+      <c r="N60" s="58"/>
     </row>
   </sheetData>
-  <mergeCells count="79">
-    <mergeCell ref="L46:N46"/>
-    <mergeCell ref="L50:N50"/>
-    <mergeCell ref="L51:N51"/>
-    <mergeCell ref="D50:K50"/>
-    <mergeCell ref="D51:K51"/>
-    <mergeCell ref="C46:K46"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="E37:H37"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B26"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="A41:G44"/>
-    <mergeCell ref="H40:K40"/>
-    <mergeCell ref="H41:K44"/>
-    <mergeCell ref="L41:N44"/>
-    <mergeCell ref="L40:N40"/>
-    <mergeCell ref="A40:G40"/>
+  <mergeCells count="78">
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="I7:N8"/>
+    <mergeCell ref="D12:K12"/>
+    <mergeCell ref="D11:K11"/>
+    <mergeCell ref="L18:N18"/>
+    <mergeCell ref="E35:H35"/>
+    <mergeCell ref="E36:H36"/>
+    <mergeCell ref="K34:N34"/>
+    <mergeCell ref="K35:N35"/>
+    <mergeCell ref="K25:N25"/>
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="K27:N27"/>
+    <mergeCell ref="K22:N22"/>
+    <mergeCell ref="K23:N24"/>
+    <mergeCell ref="D19:N21"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="L38:N38"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="F15:G17"/>
+    <mergeCell ref="H15:K17"/>
+    <mergeCell ref="L15:N17"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="K56:L59"/>
+    <mergeCell ref="M56:N59"/>
+    <mergeCell ref="K60:L60"/>
+    <mergeCell ref="M60:N60"/>
+    <mergeCell ref="H55:I55"/>
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="D52:K52"/>
     <mergeCell ref="A54:B54"/>
@@ -1853,46 +1901,30 @@
     <mergeCell ref="F60:G60"/>
     <mergeCell ref="H56:I59"/>
     <mergeCell ref="H60:I60"/>
-    <mergeCell ref="K56:L59"/>
-    <mergeCell ref="M56:N59"/>
-    <mergeCell ref="K60:L60"/>
-    <mergeCell ref="M60:N60"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="L38:N38"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="F15:G17"/>
-    <mergeCell ref="H15:K17"/>
-    <mergeCell ref="L15:N17"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E26"/>
-    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="A41:G44"/>
+    <mergeCell ref="H40:K40"/>
+    <mergeCell ref="H41:K44"/>
+    <mergeCell ref="L41:N44"/>
+    <mergeCell ref="L40:N40"/>
+    <mergeCell ref="A40:G40"/>
+    <mergeCell ref="E37:H37"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B26"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:K18"/>
     <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="L18:N18"/>
-    <mergeCell ref="E35:H35"/>
-    <mergeCell ref="E36:H36"/>
-    <mergeCell ref="K34:N34"/>
-    <mergeCell ref="K35:N35"/>
-    <mergeCell ref="D20:N20"/>
-    <mergeCell ref="K25:N25"/>
-    <mergeCell ref="K26:N26"/>
-    <mergeCell ref="K27:N27"/>
-    <mergeCell ref="K22:N22"/>
-    <mergeCell ref="K24:N24"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="I7:N8"/>
+    <mergeCell ref="C38:H38"/>
+    <mergeCell ref="L46:N46"/>
+    <mergeCell ref="L50:N50"/>
+    <mergeCell ref="L51:N51"/>
+    <mergeCell ref="D50:K50"/>
+    <mergeCell ref="D51:K51"/>
+    <mergeCell ref="C46:K47"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0" bottom="0" header="0" footer="0.3"/>

</xml_diff>

<commit_message>
dev-3.0 : print nama
</commit_message>
<xml_diff>
--- a/storage/template/tandaterima.xlsx
+++ b/storage/template/tandaterima.xlsx
@@ -491,13 +491,25 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -515,57 +527,72 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -576,51 +603,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -998,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38:H38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27:N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1025,12 +1025,12 @@
       <c r="J5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="49" t="s">
+      <c r="K5" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="49"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="49"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
       <c r="O5" s="27"/>
     </row>
     <row r="6" spans="1:15" ht="15.75">
@@ -1040,32 +1040,32 @@
       <c r="J6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="67"/>
-      <c r="L6" s="67"/>
-      <c r="M6" s="67"/>
-      <c r="N6" s="67"/>
+      <c r="K6" s="79"/>
+      <c r="L6" s="79"/>
+      <c r="M6" s="79"/>
+      <c r="N6" s="79"/>
     </row>
     <row r="7" spans="1:15" ht="17.25">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="69"/>
-      <c r="N7" s="69"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="80"/>
+      <c r="L7" s="80"/>
+      <c r="M7" s="80"/>
+      <c r="N7" s="80"/>
     </row>
     <row r="8" spans="1:15" ht="17.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="69"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69"/>
-      <c r="L8" s="69"/>
-      <c r="M8" s="69"/>
-      <c r="N8" s="69"/>
+      <c r="I8" s="80"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="80"/>
+      <c r="M8" s="80"/>
+      <c r="N8" s="80"/>
     </row>
     <row r="9" spans="1:15" ht="17.25">
       <c r="A9" s="1" t="s">
@@ -1077,10 +1077,10 @@
       <c r="J9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="49"/>
-      <c r="L9" s="49"/>
-      <c r="M9" s="49"/>
-      <c r="N9" s="49"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="63"/>
+      <c r="N9" s="63"/>
     </row>
     <row r="10" spans="1:15" ht="16.5" customHeight="1">
       <c r="F10" s="5" t="s">
@@ -1088,39 +1088,39 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="17.25">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="49"/>
+      <c r="B11" s="63"/>
       <c r="C11" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="68"/>
-      <c r="E11" s="68"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="68"/>
-      <c r="H11" s="68"/>
-      <c r="I11" s="68"/>
-      <c r="J11" s="68"/>
-      <c r="K11" s="68"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="81"/>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:15" ht="17.25">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="49"/>
+      <c r="B12" s="63"/>
       <c r="C12" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="68"/>
-      <c r="E12" s="68"/>
-      <c r="F12" s="68"/>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="68"/>
-      <c r="K12" s="68"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="81"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="81"/>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1">
@@ -1141,93 +1141,93 @@
       <c r="A14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="61" t="s">
+      <c r="B14" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61" t="s">
+      <c r="C14" s="71"/>
+      <c r="D14" s="71"/>
+      <c r="E14" s="71"/>
+      <c r="F14" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="G14" s="61"/>
-      <c r="H14" s="61" t="s">
+      <c r="G14" s="71"/>
+      <c r="H14" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="61"/>
-      <c r="J14" s="61"/>
-      <c r="K14" s="61"/>
-      <c r="L14" s="61" t="s">
+      <c r="I14" s="71"/>
+      <c r="J14" s="71"/>
+      <c r="K14" s="71"/>
+      <c r="L14" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="M14" s="61"/>
-      <c r="N14" s="61"/>
+      <c r="M14" s="71"/>
+      <c r="N14" s="71"/>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="48">
+      <c r="A15" s="62">
         <v>1</v>
       </c>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="48"/>
-      <c r="L15" s="48"/>
-      <c r="M15" s="48"/>
-      <c r="N15" s="48"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="62"/>
+      <c r="J15" s="62"/>
+      <c r="K15" s="62"/>
+      <c r="L15" s="62"/>
+      <c r="M15" s="62"/>
+      <c r="N15" s="62"/>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="48"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="48"/>
-      <c r="L16" s="48"/>
-      <c r="M16" s="48"/>
-      <c r="N16" s="48"/>
+      <c r="A16" s="62"/>
+      <c r="B16" s="62"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="62"/>
+      <c r="I16" s="62"/>
+      <c r="J16" s="62"/>
+      <c r="K16" s="62"/>
+      <c r="L16" s="62"/>
+      <c r="M16" s="62"/>
+      <c r="N16" s="62"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="48"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="48"/>
-      <c r="L17" s="48"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="48"/>
+      <c r="A17" s="62"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="62"/>
+      <c r="I17" s="62"/>
+      <c r="J17" s="62"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="62"/>
+      <c r="N17" s="62"/>
     </row>
     <row r="18" spans="1:14" ht="17.25">
       <c r="A18" s="6"/>
-      <c r="B18" s="52"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="52"/>
-      <c r="I18" s="52"/>
-      <c r="J18" s="52"/>
-      <c r="K18" s="52"/>
-      <c r="L18" s="48"/>
-      <c r="M18" s="48"/>
-      <c r="N18" s="48"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="66"/>
+      <c r="H18" s="66"/>
+      <c r="I18" s="66"/>
+      <c r="J18" s="66"/>
+      <c r="K18" s="66"/>
+      <c r="L18" s="62"/>
+      <c r="M18" s="62"/>
+      <c r="N18" s="62"/>
     </row>
     <row r="19" spans="1:14" ht="6.75" customHeight="1">
       <c r="A19" s="1"/>
@@ -1246,10 +1246,10 @@
       <c r="N19" s="77"/>
     </row>
     <row r="20" spans="1:14" ht="15.75">
-      <c r="A20" s="49" t="s">
+      <c r="A20" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="49"/>
+      <c r="B20" s="63"/>
       <c r="C20" s="24" t="s">
         <v>5</v>
       </c>
@@ -1282,32 +1282,32 @@
       <c r="N21" s="78"/>
     </row>
     <row r="22" spans="1:14" ht="17.25">
-      <c r="A22" s="51" t="s">
+      <c r="A22" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51" t="s">
+      <c r="B22" s="65"/>
+      <c r="C22" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="51"/>
-      <c r="E22" s="51"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
       <c r="F22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="7" t="s">
         <v>17</v>
       </c>
       <c r="J22" s="1"/>
-      <c r="K22" s="66"/>
-      <c r="L22" s="66"/>
-      <c r="M22" s="66"/>
-      <c r="N22" s="66"/>
+      <c r="K22" s="76"/>
+      <c r="L22" s="76"/>
+      <c r="M22" s="76"/>
+      <c r="N22" s="76"/>
     </row>
     <row r="23" spans="1:14" ht="15.75">
-      <c r="A23" s="50"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
+      <c r="A23" s="64"/>
+      <c r="B23" s="64"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="64"/>
       <c r="G23" s="7" t="s">
         <v>18</v>
       </c>
@@ -1315,28 +1315,28 @@
       <c r="J23" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K23" s="72"/>
-      <c r="L23" s="72"/>
-      <c r="M23" s="72"/>
-      <c r="N23" s="72"/>
+      <c r="K23" s="75"/>
+      <c r="L23" s="75"/>
+      <c r="M23" s="75"/>
+      <c r="N23" s="75"/>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A24" s="50"/>
-      <c r="B24" s="50"/>
-      <c r="C24" s="50"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50"/>
-      <c r="K24" s="72"/>
-      <c r="L24" s="72"/>
-      <c r="M24" s="72"/>
-      <c r="N24" s="72"/>
+      <c r="A24" s="64"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="64"/>
+      <c r="K24" s="75"/>
+      <c r="L24" s="75"/>
+      <c r="M24" s="75"/>
+      <c r="N24" s="75"/>
     </row>
     <row r="25" spans="1:14" ht="15.75">
-      <c r="A25" s="50"/>
-      <c r="B25" s="50"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
+      <c r="A25" s="64"/>
+      <c r="B25" s="64"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="64"/>
       <c r="G25" s="7" t="s">
         <v>19</v>
       </c>
@@ -1344,17 +1344,17 @@
       <c r="J25" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K25" s="65"/>
-      <c r="L25" s="65"/>
-      <c r="M25" s="65"/>
-      <c r="N25" s="65"/>
+      <c r="K25" s="74"/>
+      <c r="L25" s="74"/>
+      <c r="M25" s="74"/>
+      <c r="N25" s="74"/>
     </row>
     <row r="26" spans="1:14" ht="15.75">
-      <c r="A26" s="50"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
+      <c r="A26" s="64"/>
+      <c r="B26" s="64"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="64"/>
       <c r="G26" s="7" t="s">
         <v>20</v>
       </c>
@@ -1362,17 +1362,17 @@
       <c r="J26" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K26" s="65"/>
-      <c r="L26" s="65"/>
-      <c r="M26" s="65"/>
-      <c r="N26" s="65"/>
+      <c r="K26" s="74"/>
+      <c r="L26" s="74"/>
+      <c r="M26" s="74"/>
+      <c r="N26" s="74"/>
     </row>
     <row r="27" spans="1:14" ht="15.75">
-      <c r="A27" s="50"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
+      <c r="A27" s="64"/>
+      <c r="B27" s="64"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="65"/>
       <c r="G27" s="7" t="s">
         <v>21</v>
       </c>
@@ -1380,10 +1380,10 @@
       <c r="J27" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K27" s="65"/>
-      <c r="L27" s="65"/>
-      <c r="M27" s="65"/>
-      <c r="N27" s="65"/>
+      <c r="K27" s="74"/>
+      <c r="L27" s="74"/>
+      <c r="M27" s="74"/>
+      <c r="N27" s="74"/>
     </row>
     <row r="29" spans="1:14" ht="40.5" customHeight="1"/>
     <row r="31" spans="1:14">
@@ -1440,64 +1440,64 @@
       <c r="J34" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K34" s="64"/>
-      <c r="L34" s="64"/>
-      <c r="M34" s="64"/>
-      <c r="N34" s="64"/>
+      <c r="K34" s="73"/>
+      <c r="L34" s="73"/>
+      <c r="M34" s="73"/>
+      <c r="N34" s="73"/>
     </row>
     <row r="35" spans="1:14">
       <c r="A35" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D35" s="12"/>
-      <c r="E35" s="63" t="s">
+      <c r="E35" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="F35" s="63"/>
-      <c r="G35" s="63"/>
-      <c r="H35" s="63"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="72"/>
+      <c r="H35" s="72"/>
       <c r="I35" s="9" t="s">
         <v>25</v>
       </c>
       <c r="J35" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K35" s="64"/>
-      <c r="L35" s="64"/>
-      <c r="M35" s="64"/>
-      <c r="N35" s="64"/>
+      <c r="K35" s="73"/>
+      <c r="L35" s="73"/>
+      <c r="M35" s="73"/>
+      <c r="N35" s="73"/>
     </row>
     <row r="36" spans="1:14">
-      <c r="E36" s="63" t="s">
+      <c r="E36" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="F36" s="63"/>
-      <c r="G36" s="63"/>
-      <c r="H36" s="63"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="72"/>
+      <c r="H36" s="72"/>
     </row>
     <row r="37" spans="1:14" ht="18" customHeight="1">
       <c r="D37" s="26"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="47"/>
-      <c r="H37" s="47"/>
+      <c r="E37" s="61"/>
+      <c r="F37" s="61"/>
+      <c r="G37" s="61"/>
+      <c r="H37" s="61"/>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="62" t="s">
+      <c r="A38" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="62"/>
-      <c r="C38" s="79"/>
-      <c r="D38" s="80"/>
-      <c r="E38" s="80"/>
-      <c r="F38" s="80"/>
-      <c r="G38" s="80"/>
-      <c r="H38" s="81"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="40"/>
+      <c r="H38" s="41"/>
       <c r="I38" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="J38" s="46"/>
-      <c r="K38" s="46"/>
+      <c r="J38" s="70"/>
+      <c r="K38" s="70"/>
       <c r="L38" s="59"/>
       <c r="M38" s="59"/>
       <c r="N38" s="60"/>
@@ -1506,122 +1506,122 @@
       <c r="J39" s="19"/>
     </row>
     <row r="40" spans="1:14">
-      <c r="A40" s="53" t="s">
+      <c r="A40" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="53"/>
-      <c r="C40" s="53"/>
-      <c r="D40" s="53"/>
-      <c r="E40" s="53"/>
-      <c r="F40" s="53"/>
-      <c r="G40" s="53"/>
-      <c r="H40" s="53" t="s">
+      <c r="B40" s="55"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="55"/>
+      <c r="E40" s="55"/>
+      <c r="F40" s="55"/>
+      <c r="G40" s="55"/>
+      <c r="H40" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="I40" s="53"/>
-      <c r="J40" s="53"/>
-      <c r="K40" s="53"/>
-      <c r="L40" s="53" t="s">
+      <c r="I40" s="55"/>
+      <c r="J40" s="55"/>
+      <c r="K40" s="55"/>
+      <c r="L40" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="M40" s="53"/>
-      <c r="N40" s="53"/>
+      <c r="M40" s="55"/>
+      <c r="N40" s="55"/>
     </row>
     <row r="41" spans="1:14">
-      <c r="A41" s="70"/>
-      <c r="B41" s="70"/>
-      <c r="C41" s="70"/>
-      <c r="D41" s="70"/>
-      <c r="E41" s="70"/>
-      <c r="F41" s="70"/>
-      <c r="G41" s="70"/>
-      <c r="H41" s="70"/>
-      <c r="I41" s="70"/>
-      <c r="J41" s="70"/>
-      <c r="K41" s="70"/>
-      <c r="L41" s="71"/>
-      <c r="M41" s="71"/>
-      <c r="N41" s="71"/>
+      <c r="A41" s="54"/>
+      <c r="B41" s="54"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="54"/>
+      <c r="F41" s="54"/>
+      <c r="G41" s="54"/>
+      <c r="H41" s="54"/>
+      <c r="I41" s="54"/>
+      <c r="J41" s="54"/>
+      <c r="K41" s="54"/>
+      <c r="L41" s="56"/>
+      <c r="M41" s="56"/>
+      <c r="N41" s="56"/>
     </row>
     <row r="42" spans="1:14">
-      <c r="A42" s="70"/>
-      <c r="B42" s="70"/>
-      <c r="C42" s="70"/>
-      <c r="D42" s="70"/>
-      <c r="E42" s="70"/>
-      <c r="F42" s="70"/>
-      <c r="G42" s="70"/>
-      <c r="H42" s="70"/>
-      <c r="I42" s="70"/>
-      <c r="J42" s="70"/>
-      <c r="K42" s="70"/>
-      <c r="L42" s="71"/>
-      <c r="M42" s="71"/>
-      <c r="N42" s="71"/>
+      <c r="A42" s="54"/>
+      <c r="B42" s="54"/>
+      <c r="C42" s="54"/>
+      <c r="D42" s="54"/>
+      <c r="E42" s="54"/>
+      <c r="F42" s="54"/>
+      <c r="G42" s="54"/>
+      <c r="H42" s="54"/>
+      <c r="I42" s="54"/>
+      <c r="J42" s="54"/>
+      <c r="K42" s="54"/>
+      <c r="L42" s="56"/>
+      <c r="M42" s="56"/>
+      <c r="N42" s="56"/>
     </row>
     <row r="43" spans="1:14">
-      <c r="A43" s="70"/>
-      <c r="B43" s="70"/>
-      <c r="C43" s="70"/>
-      <c r="D43" s="70"/>
-      <c r="E43" s="70"/>
-      <c r="F43" s="70"/>
-      <c r="G43" s="70"/>
-      <c r="H43" s="70"/>
-      <c r="I43" s="70"/>
-      <c r="J43" s="70"/>
-      <c r="K43" s="70"/>
-      <c r="L43" s="71"/>
-      <c r="M43" s="71"/>
-      <c r="N43" s="71"/>
+      <c r="A43" s="54"/>
+      <c r="B43" s="54"/>
+      <c r="C43" s="54"/>
+      <c r="D43" s="54"/>
+      <c r="E43" s="54"/>
+      <c r="F43" s="54"/>
+      <c r="G43" s="54"/>
+      <c r="H43" s="54"/>
+      <c r="I43" s="54"/>
+      <c r="J43" s="54"/>
+      <c r="K43" s="54"/>
+      <c r="L43" s="56"/>
+      <c r="M43" s="56"/>
+      <c r="N43" s="56"/>
     </row>
     <row r="44" spans="1:14">
-      <c r="A44" s="70"/>
-      <c r="B44" s="70"/>
-      <c r="C44" s="70"/>
-      <c r="D44" s="70"/>
-      <c r="E44" s="70"/>
-      <c r="F44" s="70"/>
-      <c r="G44" s="70"/>
-      <c r="H44" s="70"/>
-      <c r="I44" s="70"/>
-      <c r="J44" s="70"/>
-      <c r="K44" s="70"/>
-      <c r="L44" s="71"/>
-      <c r="M44" s="71"/>
-      <c r="N44" s="71"/>
+      <c r="A44" s="54"/>
+      <c r="B44" s="54"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="54"/>
+      <c r="F44" s="54"/>
+      <c r="G44" s="54"/>
+      <c r="H44" s="54"/>
+      <c r="I44" s="54"/>
+      <c r="J44" s="54"/>
+      <c r="K44" s="54"/>
+      <c r="L44" s="56"/>
+      <c r="M44" s="56"/>
+      <c r="N44" s="56"/>
     </row>
     <row r="45" spans="1:14" ht="3.75" customHeight="1"/>
     <row r="46" spans="1:14">
-      <c r="A46" s="54" t="s">
+      <c r="A46" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="55"/>
-      <c r="C46" s="73"/>
-      <c r="D46" s="73"/>
-      <c r="E46" s="73"/>
-      <c r="F46" s="73"/>
-      <c r="G46" s="73"/>
-      <c r="H46" s="73"/>
-      <c r="I46" s="73"/>
-      <c r="J46" s="73"/>
-      <c r="K46" s="74"/>
-      <c r="L46" s="38"/>
-      <c r="M46" s="39"/>
-      <c r="N46" s="40"/>
+      <c r="B46" s="58"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="50"/>
+      <c r="E46" s="50"/>
+      <c r="F46" s="50"/>
+      <c r="G46" s="50"/>
+      <c r="H46" s="50"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="50"/>
+      <c r="K46" s="51"/>
+      <c r="L46" s="42"/>
+      <c r="M46" s="43"/>
+      <c r="N46" s="44"/>
     </row>
     <row r="47" spans="1:14" ht="15" customHeight="1">
       <c r="A47" s="14"/>
       <c r="B47" s="15"/>
-      <c r="C47" s="75"/>
-      <c r="D47" s="75"/>
-      <c r="E47" s="75"/>
-      <c r="F47" s="75"/>
-      <c r="G47" s="75"/>
-      <c r="H47" s="75"/>
-      <c r="I47" s="75"/>
-      <c r="J47" s="75"/>
-      <c r="K47" s="76"/>
+      <c r="C47" s="52"/>
+      <c r="D47" s="52"/>
+      <c r="E47" s="52"/>
+      <c r="F47" s="52"/>
+      <c r="G47" s="52"/>
+      <c r="H47" s="52"/>
+      <c r="I47" s="52"/>
+      <c r="J47" s="52"/>
+      <c r="K47" s="53"/>
       <c r="L47" s="14"/>
       <c r="M47" s="15"/>
       <c r="N47" s="16"/>
@@ -1650,19 +1650,19 @@
       <c r="C50" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D50" s="42"/>
-      <c r="E50" s="42"/>
-      <c r="F50" s="42"/>
-      <c r="G50" s="42"/>
-      <c r="H50" s="42"/>
-      <c r="I50" s="42"/>
-      <c r="J50" s="42"/>
-      <c r="K50" s="43"/>
-      <c r="L50" s="41" t="s">
+      <c r="D50" s="46"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="46"/>
+      <c r="I50" s="46"/>
+      <c r="J50" s="46"/>
+      <c r="K50" s="47"/>
+      <c r="L50" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="M50" s="41"/>
-      <c r="N50" s="41"/>
+      <c r="M50" s="45"/>
+      <c r="N50" s="45"/>
       <c r="O50" s="11"/>
     </row>
     <row r="51" spans="1:15">
@@ -1673,17 +1673,17 @@
       <c r="C51" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D51" s="44"/>
-      <c r="E51" s="44"/>
-      <c r="F51" s="44"/>
-      <c r="G51" s="44"/>
-      <c r="H51" s="44"/>
-      <c r="I51" s="44"/>
-      <c r="J51" s="44"/>
-      <c r="K51" s="45"/>
-      <c r="L51" s="41"/>
-      <c r="M51" s="41"/>
-      <c r="N51" s="41"/>
+      <c r="D51" s="48"/>
+      <c r="E51" s="48"/>
+      <c r="F51" s="48"/>
+      <c r="G51" s="48"/>
+      <c r="H51" s="48"/>
+      <c r="I51" s="48"/>
+      <c r="J51" s="48"/>
+      <c r="K51" s="49"/>
+      <c r="L51" s="45"/>
+      <c r="M51" s="45"/>
+      <c r="N51" s="45"/>
     </row>
     <row r="52" spans="1:15" ht="15" customHeight="1">
       <c r="A52" s="31" t="s">
@@ -1693,157 +1693,157 @@
       <c r="C52" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D52" s="56"/>
-      <c r="E52" s="56"/>
-      <c r="F52" s="56"/>
-      <c r="G52" s="56"/>
-      <c r="H52" s="56"/>
-      <c r="I52" s="56"/>
-      <c r="J52" s="56"/>
-      <c r="K52" s="57"/>
+      <c r="D52" s="67"/>
+      <c r="E52" s="67"/>
+      <c r="F52" s="67"/>
+      <c r="G52" s="67"/>
+      <c r="H52" s="67"/>
+      <c r="I52" s="67"/>
+      <c r="J52" s="67"/>
+      <c r="K52" s="68"/>
     </row>
     <row r="53" spans="1:15" ht="4.5" customHeight="1"/>
     <row r="54" spans="1:15">
-      <c r="A54" s="58" t="s">
+      <c r="A54" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="B54" s="58"/>
+      <c r="B54" s="69"/>
       <c r="C54" s="10"/>
-      <c r="D54" s="58" t="s">
+      <c r="D54" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="E54" s="58"/>
-      <c r="F54" s="58"/>
-      <c r="G54" s="58"/>
-      <c r="H54" s="58"/>
-      <c r="I54" s="58"/>
+      <c r="E54" s="69"/>
+      <c r="F54" s="69"/>
+      <c r="G54" s="69"/>
+      <c r="H54" s="69"/>
+      <c r="I54" s="69"/>
       <c r="J54" s="10"/>
-      <c r="K54" s="58" t="s">
+      <c r="K54" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="L54" s="58"/>
-      <c r="M54" s="58"/>
-      <c r="N54" s="58"/>
+      <c r="L54" s="69"/>
+      <c r="M54" s="69"/>
+      <c r="N54" s="69"/>
     </row>
     <row r="55" spans="1:15">
-      <c r="A55" s="58" t="s">
+      <c r="A55" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="B55" s="58"/>
+      <c r="B55" s="69"/>
       <c r="C55" s="10"/>
-      <c r="D55" s="58" t="s">
+      <c r="D55" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="E55" s="58"/>
-      <c r="F55" s="58" t="s">
+      <c r="E55" s="69"/>
+      <c r="F55" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="G55" s="58"/>
-      <c r="H55" s="58" t="s">
+      <c r="G55" s="69"/>
+      <c r="H55" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="I55" s="58"/>
+      <c r="I55" s="69"/>
       <c r="J55" s="25"/>
-      <c r="K55" s="58" t="s">
+      <c r="K55" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="L55" s="58"/>
-      <c r="M55" s="58" t="s">
+      <c r="L55" s="69"/>
+      <c r="M55" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="N55" s="58"/>
+      <c r="N55" s="69"/>
     </row>
     <row r="56" spans="1:15">
-      <c r="A56" s="58"/>
-      <c r="B56" s="58"/>
+      <c r="A56" s="69"/>
+      <c r="B56" s="69"/>
       <c r="C56" s="10"/>
-      <c r="D56" s="58"/>
-      <c r="E56" s="58"/>
-      <c r="F56" s="58"/>
-      <c r="G56" s="58"/>
-      <c r="H56" s="58"/>
-      <c r="I56" s="58"/>
+      <c r="D56" s="69"/>
+      <c r="E56" s="69"/>
+      <c r="F56" s="69"/>
+      <c r="G56" s="69"/>
+      <c r="H56" s="69"/>
+      <c r="I56" s="69"/>
       <c r="J56" s="10"/>
-      <c r="K56" s="58"/>
-      <c r="L56" s="58"/>
-      <c r="M56" s="58"/>
-      <c r="N56" s="58"/>
+      <c r="K56" s="69"/>
+      <c r="L56" s="69"/>
+      <c r="M56" s="69"/>
+      <c r="N56" s="69"/>
     </row>
     <row r="57" spans="1:15">
-      <c r="A57" s="58"/>
-      <c r="B57" s="58"/>
+      <c r="A57" s="69"/>
+      <c r="B57" s="69"/>
       <c r="C57" s="10"/>
-      <c r="D57" s="58"/>
-      <c r="E57" s="58"/>
-      <c r="F57" s="58"/>
-      <c r="G57" s="58"/>
-      <c r="H57" s="58"/>
-      <c r="I57" s="58"/>
+      <c r="D57" s="69"/>
+      <c r="E57" s="69"/>
+      <c r="F57" s="69"/>
+      <c r="G57" s="69"/>
+      <c r="H57" s="69"/>
+      <c r="I57" s="69"/>
       <c r="J57" s="10"/>
-      <c r="K57" s="58"/>
-      <c r="L57" s="58"/>
-      <c r="M57" s="58"/>
-      <c r="N57" s="58"/>
+      <c r="K57" s="69"/>
+      <c r="L57" s="69"/>
+      <c r="M57" s="69"/>
+      <c r="N57" s="69"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="58"/>
-      <c r="B58" s="58"/>
+      <c r="A58" s="69"/>
+      <c r="B58" s="69"/>
       <c r="C58" s="10"/>
-      <c r="D58" s="58"/>
-      <c r="E58" s="58"/>
-      <c r="F58" s="58"/>
-      <c r="G58" s="58"/>
-      <c r="H58" s="58"/>
-      <c r="I58" s="58"/>
+      <c r="D58" s="69"/>
+      <c r="E58" s="69"/>
+      <c r="F58" s="69"/>
+      <c r="G58" s="69"/>
+      <c r="H58" s="69"/>
+      <c r="I58" s="69"/>
       <c r="J58" s="10"/>
-      <c r="K58" s="58"/>
-      <c r="L58" s="58"/>
-      <c r="M58" s="58"/>
-      <c r="N58" s="58"/>
+      <c r="K58" s="69"/>
+      <c r="L58" s="69"/>
+      <c r="M58" s="69"/>
+      <c r="N58" s="69"/>
     </row>
     <row r="59" spans="1:15">
-      <c r="A59" s="58"/>
-      <c r="B59" s="58"/>
+      <c r="A59" s="69"/>
+      <c r="B59" s="69"/>
       <c r="C59" s="10"/>
-      <c r="D59" s="58"/>
-      <c r="E59" s="58"/>
-      <c r="F59" s="58"/>
-      <c r="G59" s="58"/>
-      <c r="H59" s="58"/>
-      <c r="I59" s="58"/>
+      <c r="D59" s="69"/>
+      <c r="E59" s="69"/>
+      <c r="F59" s="69"/>
+      <c r="G59" s="69"/>
+      <c r="H59" s="69"/>
+      <c r="I59" s="69"/>
       <c r="J59" s="10"/>
-      <c r="K59" s="58"/>
-      <c r="L59" s="58"/>
-      <c r="M59" s="58"/>
-      <c r="N59" s="58"/>
+      <c r="K59" s="69"/>
+      <c r="L59" s="69"/>
+      <c r="M59" s="69"/>
+      <c r="N59" s="69"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="58" t="s">
+      <c r="A60" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="58"/>
+      <c r="B60" s="69"/>
       <c r="C60" s="10"/>
-      <c r="D60" s="58" t="s">
+      <c r="D60" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="E60" s="58"/>
-      <c r="F60" s="58" t="s">
+      <c r="E60" s="69"/>
+      <c r="F60" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="G60" s="58"/>
-      <c r="H60" s="58" t="s">
+      <c r="G60" s="69"/>
+      <c r="H60" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="I60" s="58"/>
+      <c r="I60" s="69"/>
       <c r="J60" s="10"/>
-      <c r="K60" s="58" t="s">
+      <c r="K60" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="L60" s="58"/>
-      <c r="M60" s="58" t="s">
+      <c r="L60" s="69"/>
+      <c r="M60" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="N60" s="58"/>
+      <c r="N60" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="78">
@@ -1853,7 +1853,22 @@
     <mergeCell ref="I7:N8"/>
     <mergeCell ref="D12:K12"/>
     <mergeCell ref="D11:K11"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="F15:G17"/>
+    <mergeCell ref="H15:K17"/>
+    <mergeCell ref="L15:N17"/>
+    <mergeCell ref="C22:E22"/>
     <mergeCell ref="L18:N18"/>
+    <mergeCell ref="K22:N22"/>
+    <mergeCell ref="D19:N21"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="C23:E26"/>
+    <mergeCell ref="C27:E27"/>
     <mergeCell ref="E35:H35"/>
     <mergeCell ref="E36:H36"/>
     <mergeCell ref="K34:N34"/>
@@ -1861,31 +1876,13 @@
     <mergeCell ref="K25:N25"/>
     <mergeCell ref="K26:N26"/>
     <mergeCell ref="K27:N27"/>
-    <mergeCell ref="K22:N22"/>
     <mergeCell ref="K23:N24"/>
-    <mergeCell ref="D19:N21"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="L38:N38"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="F15:G17"/>
-    <mergeCell ref="H15:K17"/>
-    <mergeCell ref="L15:N17"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="K56:L59"/>
     <mergeCell ref="M56:N59"/>
     <mergeCell ref="K60:L60"/>
     <mergeCell ref="M60:N60"/>
     <mergeCell ref="H55:I55"/>
-    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="K55:L55"/>
     <mergeCell ref="D52:K52"/>
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="A55:B55"/>
@@ -1901,12 +1898,7 @@
     <mergeCell ref="F60:G60"/>
     <mergeCell ref="H56:I59"/>
     <mergeCell ref="H60:I60"/>
-    <mergeCell ref="A41:G44"/>
-    <mergeCell ref="H40:K40"/>
-    <mergeCell ref="H41:K44"/>
-    <mergeCell ref="L41:N44"/>
-    <mergeCell ref="L40:N40"/>
-    <mergeCell ref="A40:G40"/>
+    <mergeCell ref="K56:L59"/>
     <mergeCell ref="E37:H37"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A11:B11"/>
@@ -1925,6 +1917,14 @@
     <mergeCell ref="D50:K50"/>
     <mergeCell ref="D51:K51"/>
     <mergeCell ref="C46:K47"/>
+    <mergeCell ref="A41:G44"/>
+    <mergeCell ref="H40:K40"/>
+    <mergeCell ref="H41:K44"/>
+    <mergeCell ref="L41:N44"/>
+    <mergeCell ref="L40:N40"/>
+    <mergeCell ref="A40:G40"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="L38:N38"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0" bottom="0" header="0" footer="0.3"/>

</xml_diff>

<commit_message>
hotfix-3.0.1 : add barcode di tanda terima
</commit_message>
<xml_diff>
--- a/storage/template/tandaterima.xlsx
+++ b/storage/template/tandaterima.xlsx
@@ -270,16 +270,15 @@
       <name val="Free "/>
     </font>
     <font>
-      <sz val="36"/>
-      <color theme="1"/>
-      <name val="Free 3 of 9"/>
-      <family val="3"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Free 3 of 9 Extended"/>
     </font>
   </fonts>
   <fills count="2">
@@ -491,16 +490,76 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="3" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -560,68 +619,8 @@
     <xf numFmtId="3" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -998,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27:N27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1025,12 +1024,12 @@
       <c r="J5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="63" t="s">
+      <c r="K5" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="63"/>
-      <c r="M5" s="63"/>
-      <c r="N5" s="63"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
       <c r="O5" s="27"/>
     </row>
     <row r="6" spans="1:15" ht="15.75">
@@ -1040,32 +1039,32 @@
       <c r="J6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="79"/>
-      <c r="L6" s="79"/>
-      <c r="M6" s="79"/>
-      <c r="N6" s="79"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="39"/>
     </row>
     <row r="7" spans="1:15" ht="17.25">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="80"/>
-      <c r="J7" s="80"/>
-      <c r="K7" s="80"/>
-      <c r="L7" s="80"/>
-      <c r="M7" s="80"/>
-      <c r="N7" s="80"/>
+      <c r="I7" s="81"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="81"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="81"/>
+      <c r="N7" s="81"/>
     </row>
     <row r="8" spans="1:15" ht="17.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="80"/>
-      <c r="J8" s="80"/>
-      <c r="K8" s="80"/>
-      <c r="L8" s="80"/>
-      <c r="M8" s="80"/>
-      <c r="N8" s="80"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="81"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="81"/>
+      <c r="N8" s="81"/>
     </row>
     <row r="9" spans="1:15" ht="17.25">
       <c r="A9" s="1" t="s">
@@ -1077,10 +1076,10 @@
       <c r="J9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="63"/>
-      <c r="L9" s="63"/>
-      <c r="M9" s="63"/>
-      <c r="N9" s="63"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
     </row>
     <row r="10" spans="1:15" ht="16.5" customHeight="1">
       <c r="F10" s="5" t="s">
@@ -1088,39 +1087,39 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="17.25">
-      <c r="A11" s="63" t="s">
+      <c r="A11" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="63"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="81"/>
-      <c r="E11" s="81"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="81"/>
-      <c r="I11" s="81"/>
-      <c r="J11" s="81"/>
-      <c r="K11" s="81"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:15" ht="17.25">
-      <c r="A12" s="63" t="s">
+      <c r="A12" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="63"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="81"/>
-      <c r="E12" s="81"/>
-      <c r="F12" s="81"/>
-      <c r="G12" s="81"/>
-      <c r="H12" s="81"/>
-      <c r="I12" s="81"/>
-      <c r="J12" s="81"/>
-      <c r="K12" s="81"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="40"/>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1">
@@ -1141,173 +1140,173 @@
       <c r="A14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="71" t="s">
+      <c r="B14" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="71"/>
-      <c r="D14" s="71"/>
-      <c r="E14" s="71"/>
-      <c r="F14" s="71" t="s">
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="G14" s="71"/>
-      <c r="H14" s="71" t="s">
+      <c r="G14" s="41"/>
+      <c r="H14" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="71"/>
-      <c r="J14" s="71"/>
-      <c r="K14" s="71"/>
-      <c r="L14" s="71" t="s">
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="M14" s="71"/>
-      <c r="N14" s="71"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41"/>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="62">
+      <c r="A15" s="42">
         <v>1</v>
       </c>
-      <c r="B15" s="62"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="62"/>
-      <c r="I15" s="62"/>
-      <c r="J15" s="62"/>
-      <c r="K15" s="62"/>
-      <c r="L15" s="62"/>
-      <c r="M15" s="62"/>
-      <c r="N15" s="62"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="42"/>
+      <c r="N15" s="42"/>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="62"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="62"/>
-      <c r="I16" s="62"/>
-      <c r="J16" s="62"/>
-      <c r="K16" s="62"/>
-      <c r="L16" s="62"/>
-      <c r="M16" s="62"/>
-      <c r="N16" s="62"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="42"/>
+      <c r="N16" s="42"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="62"/>
-      <c r="B17" s="62"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="62"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="62"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="62"/>
-      <c r="K17" s="62"/>
-      <c r="L17" s="62"/>
-      <c r="M17" s="62"/>
-      <c r="N17" s="62"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="42"/>
+      <c r="N17" s="42"/>
     </row>
     <row r="18" spans="1:14" ht="17.25">
       <c r="A18" s="6"/>
-      <c r="B18" s="66"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="66"/>
-      <c r="H18" s="66"/>
-      <c r="I18" s="66"/>
-      <c r="J18" s="66"/>
-      <c r="K18" s="66"/>
-      <c r="L18" s="62"/>
-      <c r="M18" s="62"/>
-      <c r="N18" s="62"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="48"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="42"/>
+      <c r="N18" s="42"/>
     </row>
     <row r="19" spans="1:14" ht="6.75" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
-      <c r="D19" s="77"/>
-      <c r="E19" s="77"/>
-      <c r="F19" s="77"/>
-      <c r="G19" s="77"/>
-      <c r="H19" s="77"/>
-      <c r="I19" s="77"/>
-      <c r="J19" s="77"/>
-      <c r="K19" s="77"/>
-      <c r="L19" s="77"/>
-      <c r="M19" s="77"/>
-      <c r="N19" s="77"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="45"/>
+      <c r="M19" s="45"/>
+      <c r="N19" s="45"/>
     </row>
     <row r="20" spans="1:14" ht="15.75">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="63"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="78"/>
-      <c r="E20" s="78"/>
-      <c r="F20" s="78"/>
-      <c r="G20" s="78"/>
-      <c r="H20" s="78"/>
-      <c r="I20" s="78"/>
-      <c r="J20" s="78"/>
-      <c r="K20" s="78"/>
-      <c r="L20" s="78"/>
-      <c r="M20" s="78"/>
-      <c r="N20" s="78"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="46"/>
+      <c r="M20" s="46"/>
+      <c r="N20" s="46"/>
     </row>
     <row r="21" spans="1:14" ht="6.75" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="78"/>
-      <c r="E21" s="78"/>
-      <c r="F21" s="78"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="78"/>
-      <c r="I21" s="78"/>
-      <c r="J21" s="78"/>
-      <c r="K21" s="78"/>
-      <c r="L21" s="78"/>
-      <c r="M21" s="78"/>
-      <c r="N21" s="78"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="46"/>
     </row>
     <row r="22" spans="1:14" ht="17.25">
-      <c r="A22" s="65" t="s">
+      <c r="A22" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="65"/>
-      <c r="C22" s="65" t="s">
+      <c r="B22" s="43"/>
+      <c r="C22" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="65"/>
-      <c r="E22" s="65"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
       <c r="F22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="7" t="s">
         <v>17</v>
       </c>
       <c r="J22" s="1"/>
-      <c r="K22" s="76"/>
-      <c r="L22" s="76"/>
-      <c r="M22" s="76"/>
-      <c r="N22" s="76"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="44"/>
     </row>
     <row r="23" spans="1:14" ht="15.75">
-      <c r="A23" s="64"/>
-      <c r="B23" s="64"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
+      <c r="A23" s="49"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
       <c r="G23" s="7" t="s">
         <v>18</v>
       </c>
@@ -1315,28 +1314,28 @@
       <c r="J23" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K23" s="75"/>
-      <c r="L23" s="75"/>
-      <c r="M23" s="75"/>
-      <c r="N23" s="75"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="53"/>
+      <c r="M23" s="53"/>
+      <c r="N23" s="53"/>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A24" s="64"/>
-      <c r="B24" s="64"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
-      <c r="K24" s="75"/>
-      <c r="L24" s="75"/>
-      <c r="M24" s="75"/>
-      <c r="N24" s="75"/>
+      <c r="A24" s="49"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="K24" s="53"/>
+      <c r="L24" s="53"/>
+      <c r="M24" s="53"/>
+      <c r="N24" s="53"/>
     </row>
     <row r="25" spans="1:14" ht="15.75">
-      <c r="A25" s="64"/>
-      <c r="B25" s="64"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="64"/>
+      <c r="A25" s="49"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
       <c r="G25" s="7" t="s">
         <v>19</v>
       </c>
@@ -1344,17 +1343,17 @@
       <c r="J25" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K25" s="74"/>
-      <c r="L25" s="74"/>
-      <c r="M25" s="74"/>
-      <c r="N25" s="74"/>
+      <c r="K25" s="52"/>
+      <c r="L25" s="52"/>
+      <c r="M25" s="52"/>
+      <c r="N25" s="52"/>
     </row>
     <row r="26" spans="1:14" ht="15.75">
-      <c r="A26" s="64"/>
-      <c r="B26" s="64"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="64"/>
-      <c r="E26" s="64"/>
+      <c r="A26" s="49"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
       <c r="G26" s="7" t="s">
         <v>20</v>
       </c>
@@ -1362,17 +1361,17 @@
       <c r="J26" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K26" s="74"/>
-      <c r="L26" s="74"/>
-      <c r="M26" s="74"/>
-      <c r="N26" s="74"/>
+      <c r="K26" s="52"/>
+      <c r="L26" s="52"/>
+      <c r="M26" s="52"/>
+      <c r="N26" s="52"/>
     </row>
     <row r="27" spans="1:14" ht="15.75">
-      <c r="A27" s="64"/>
-      <c r="B27" s="64"/>
-      <c r="C27" s="65"/>
-      <c r="D27" s="65"/>
-      <c r="E27" s="65"/>
+      <c r="A27" s="49"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
       <c r="G27" s="7" t="s">
         <v>21</v>
       </c>
@@ -1380,10 +1379,10 @@
       <c r="J27" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K27" s="74"/>
-      <c r="L27" s="74"/>
-      <c r="M27" s="74"/>
-      <c r="N27" s="74"/>
+      <c r="K27" s="52"/>
+      <c r="L27" s="52"/>
+      <c r="M27" s="52"/>
+      <c r="N27" s="52"/>
     </row>
     <row r="29" spans="1:14" ht="40.5" customHeight="1"/>
     <row r="31" spans="1:14">
@@ -1440,188 +1439,188 @@
       <c r="J34" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K34" s="73"/>
-      <c r="L34" s="73"/>
-      <c r="M34" s="73"/>
-      <c r="N34" s="73"/>
+      <c r="K34" s="51"/>
+      <c r="L34" s="51"/>
+      <c r="M34" s="51"/>
+      <c r="N34" s="51"/>
     </row>
     <row r="35" spans="1:14">
       <c r="A35" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D35" s="12"/>
-      <c r="E35" s="72" t="s">
+      <c r="E35" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="F35" s="72"/>
-      <c r="G35" s="72"/>
-      <c r="H35" s="72"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
       <c r="I35" s="9" t="s">
         <v>25</v>
       </c>
       <c r="J35" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K35" s="73"/>
-      <c r="L35" s="73"/>
-      <c r="M35" s="73"/>
-      <c r="N35" s="73"/>
+      <c r="K35" s="51"/>
+      <c r="L35" s="51"/>
+      <c r="M35" s="51"/>
+      <c r="N35" s="51"/>
     </row>
     <row r="36" spans="1:14">
-      <c r="E36" s="72" t="s">
+      <c r="E36" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="F36" s="72"/>
-      <c r="G36" s="72"/>
-      <c r="H36" s="72"/>
+      <c r="F36" s="50"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="50"/>
     </row>
     <row r="37" spans="1:14" ht="18" customHeight="1">
       <c r="D37" s="26"/>
-      <c r="E37" s="61"/>
-      <c r="F37" s="61"/>
-      <c r="G37" s="61"/>
-      <c r="H37" s="61"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="57"/>
+      <c r="H37" s="57"/>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="38" t="s">
+      <c r="A38" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="38"/>
-      <c r="C38" s="39"/>
-      <c r="D38" s="40"/>
-      <c r="E38" s="40"/>
-      <c r="F38" s="40"/>
-      <c r="G38" s="40"/>
-      <c r="H38" s="41"/>
+      <c r="B38" s="58"/>
+      <c r="C38" s="59"/>
+      <c r="D38" s="60"/>
+      <c r="E38" s="60"/>
+      <c r="F38" s="60"/>
+      <c r="G38" s="60"/>
+      <c r="H38" s="61"/>
       <c r="I38" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="J38" s="70"/>
-      <c r="K38" s="70"/>
-      <c r="L38" s="59"/>
-      <c r="M38" s="59"/>
-      <c r="N38" s="60"/>
+      <c r="J38" s="47"/>
+      <c r="K38" s="47"/>
+      <c r="L38" s="79"/>
+      <c r="M38" s="79"/>
+      <c r="N38" s="80"/>
     </row>
     <row r="39" spans="1:14" ht="3.75" customHeight="1">
       <c r="J39" s="19"/>
     </row>
     <row r="40" spans="1:14">
-      <c r="A40" s="55" t="s">
+      <c r="A40" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="55"/>
-      <c r="C40" s="55"/>
-      <c r="D40" s="55"/>
-      <c r="E40" s="55"/>
-      <c r="F40" s="55"/>
-      <c r="G40" s="55"/>
-      <c r="H40" s="55" t="s">
+      <c r="B40" s="75"/>
+      <c r="C40" s="75"/>
+      <c r="D40" s="75"/>
+      <c r="E40" s="75"/>
+      <c r="F40" s="75"/>
+      <c r="G40" s="75"/>
+      <c r="H40" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="I40" s="55"/>
-      <c r="J40" s="55"/>
-      <c r="K40" s="55"/>
-      <c r="L40" s="55" t="s">
+      <c r="I40" s="75"/>
+      <c r="J40" s="75"/>
+      <c r="K40" s="75"/>
+      <c r="L40" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="M40" s="55"/>
-      <c r="N40" s="55"/>
+      <c r="M40" s="75"/>
+      <c r="N40" s="75"/>
     </row>
     <row r="41" spans="1:14">
-      <c r="A41" s="54"/>
-      <c r="B41" s="54"/>
-      <c r="C41" s="54"/>
-      <c r="D41" s="54"/>
-      <c r="E41" s="54"/>
-      <c r="F41" s="54"/>
-      <c r="G41" s="54"/>
-      <c r="H41" s="54"/>
-      <c r="I41" s="54"/>
-      <c r="J41" s="54"/>
-      <c r="K41" s="54"/>
-      <c r="L41" s="56"/>
-      <c r="M41" s="56"/>
-      <c r="N41" s="56"/>
+      <c r="A41" s="74"/>
+      <c r="B41" s="74"/>
+      <c r="C41" s="74"/>
+      <c r="D41" s="74"/>
+      <c r="E41" s="74"/>
+      <c r="F41" s="74"/>
+      <c r="G41" s="74"/>
+      <c r="H41" s="74"/>
+      <c r="I41" s="74"/>
+      <c r="J41" s="74"/>
+      <c r="K41" s="74"/>
+      <c r="L41" s="76"/>
+      <c r="M41" s="76"/>
+      <c r="N41" s="76"/>
     </row>
     <row r="42" spans="1:14">
-      <c r="A42" s="54"/>
-      <c r="B42" s="54"/>
-      <c r="C42" s="54"/>
-      <c r="D42" s="54"/>
-      <c r="E42" s="54"/>
-      <c r="F42" s="54"/>
-      <c r="G42" s="54"/>
-      <c r="H42" s="54"/>
-      <c r="I42" s="54"/>
-      <c r="J42" s="54"/>
-      <c r="K42" s="54"/>
-      <c r="L42" s="56"/>
-      <c r="M42" s="56"/>
-      <c r="N42" s="56"/>
+      <c r="A42" s="74"/>
+      <c r="B42" s="74"/>
+      <c r="C42" s="74"/>
+      <c r="D42" s="74"/>
+      <c r="E42" s="74"/>
+      <c r="F42" s="74"/>
+      <c r="G42" s="74"/>
+      <c r="H42" s="74"/>
+      <c r="I42" s="74"/>
+      <c r="J42" s="74"/>
+      <c r="K42" s="74"/>
+      <c r="L42" s="76"/>
+      <c r="M42" s="76"/>
+      <c r="N42" s="76"/>
     </row>
     <row r="43" spans="1:14">
-      <c r="A43" s="54"/>
-      <c r="B43" s="54"/>
-      <c r="C43" s="54"/>
-      <c r="D43" s="54"/>
-      <c r="E43" s="54"/>
-      <c r="F43" s="54"/>
-      <c r="G43" s="54"/>
-      <c r="H43" s="54"/>
-      <c r="I43" s="54"/>
-      <c r="J43" s="54"/>
-      <c r="K43" s="54"/>
-      <c r="L43" s="56"/>
-      <c r="M43" s="56"/>
-      <c r="N43" s="56"/>
+      <c r="A43" s="74"/>
+      <c r="B43" s="74"/>
+      <c r="C43" s="74"/>
+      <c r="D43" s="74"/>
+      <c r="E43" s="74"/>
+      <c r="F43" s="74"/>
+      <c r="G43" s="74"/>
+      <c r="H43" s="74"/>
+      <c r="I43" s="74"/>
+      <c r="J43" s="74"/>
+      <c r="K43" s="74"/>
+      <c r="L43" s="76"/>
+      <c r="M43" s="76"/>
+      <c r="N43" s="76"/>
     </row>
     <row r="44" spans="1:14">
-      <c r="A44" s="54"/>
-      <c r="B44" s="54"/>
-      <c r="C44" s="54"/>
-      <c r="D44" s="54"/>
-      <c r="E44" s="54"/>
-      <c r="F44" s="54"/>
-      <c r="G44" s="54"/>
-      <c r="H44" s="54"/>
-      <c r="I44" s="54"/>
-      <c r="J44" s="54"/>
-      <c r="K44" s="54"/>
-      <c r="L44" s="56"/>
-      <c r="M44" s="56"/>
-      <c r="N44" s="56"/>
+      <c r="A44" s="74"/>
+      <c r="B44" s="74"/>
+      <c r="C44" s="74"/>
+      <c r="D44" s="74"/>
+      <c r="E44" s="74"/>
+      <c r="F44" s="74"/>
+      <c r="G44" s="74"/>
+      <c r="H44" s="74"/>
+      <c r="I44" s="74"/>
+      <c r="J44" s="74"/>
+      <c r="K44" s="74"/>
+      <c r="L44" s="76"/>
+      <c r="M44" s="76"/>
+      <c r="N44" s="76"/>
     </row>
     <row r="45" spans="1:14" ht="3.75" customHeight="1"/>
     <row r="46" spans="1:14">
-      <c r="A46" s="57" t="s">
+      <c r="A46" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="58"/>
-      <c r="C46" s="50"/>
-      <c r="D46" s="50"/>
-      <c r="E46" s="50"/>
-      <c r="F46" s="50"/>
-      <c r="G46" s="50"/>
-      <c r="H46" s="50"/>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
-      <c r="K46" s="51"/>
-      <c r="L46" s="42"/>
-      <c r="M46" s="43"/>
-      <c r="N46" s="44"/>
+      <c r="B46" s="78"/>
+      <c r="C46" s="70"/>
+      <c r="D46" s="70"/>
+      <c r="E46" s="70"/>
+      <c r="F46" s="70"/>
+      <c r="G46" s="70"/>
+      <c r="H46" s="70"/>
+      <c r="I46" s="70"/>
+      <c r="J46" s="70"/>
+      <c r="K46" s="71"/>
+      <c r="L46" s="62"/>
+      <c r="M46" s="63"/>
+      <c r="N46" s="64"/>
     </row>
     <row r="47" spans="1:14" ht="15" customHeight="1">
       <c r="A47" s="14"/>
       <c r="B47" s="15"/>
-      <c r="C47" s="52"/>
-      <c r="D47" s="52"/>
-      <c r="E47" s="52"/>
-      <c r="F47" s="52"/>
-      <c r="G47" s="52"/>
-      <c r="H47" s="52"/>
-      <c r="I47" s="52"/>
-      <c r="J47" s="52"/>
-      <c r="K47" s="53"/>
+      <c r="C47" s="72"/>
+      <c r="D47" s="72"/>
+      <c r="E47" s="72"/>
+      <c r="F47" s="72"/>
+      <c r="G47" s="72"/>
+      <c r="H47" s="72"/>
+      <c r="I47" s="72"/>
+      <c r="J47" s="72"/>
+      <c r="K47" s="73"/>
       <c r="L47" s="14"/>
       <c r="M47" s="15"/>
       <c r="N47" s="16"/>
@@ -1650,19 +1649,19 @@
       <c r="C50" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D50" s="46"/>
-      <c r="E50" s="46"/>
-      <c r="F50" s="46"/>
-      <c r="G50" s="46"/>
-      <c r="H50" s="46"/>
-      <c r="I50" s="46"/>
-      <c r="J50" s="46"/>
-      <c r="K50" s="47"/>
-      <c r="L50" s="45" t="s">
+      <c r="D50" s="66"/>
+      <c r="E50" s="66"/>
+      <c r="F50" s="66"/>
+      <c r="G50" s="66"/>
+      <c r="H50" s="66"/>
+      <c r="I50" s="66"/>
+      <c r="J50" s="66"/>
+      <c r="K50" s="67"/>
+      <c r="L50" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="M50" s="45"/>
-      <c r="N50" s="45"/>
+      <c r="M50" s="65"/>
+      <c r="N50" s="65"/>
       <c r="O50" s="11"/>
     </row>
     <row r="51" spans="1:15">
@@ -1673,17 +1672,17 @@
       <c r="C51" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D51" s="48"/>
-      <c r="E51" s="48"/>
-      <c r="F51" s="48"/>
-      <c r="G51" s="48"/>
-      <c r="H51" s="48"/>
-      <c r="I51" s="48"/>
-      <c r="J51" s="48"/>
-      <c r="K51" s="49"/>
-      <c r="L51" s="45"/>
-      <c r="M51" s="45"/>
-      <c r="N51" s="45"/>
+      <c r="D51" s="68"/>
+      <c r="E51" s="68"/>
+      <c r="F51" s="68"/>
+      <c r="G51" s="68"/>
+      <c r="H51" s="68"/>
+      <c r="I51" s="68"/>
+      <c r="J51" s="68"/>
+      <c r="K51" s="69"/>
+      <c r="L51" s="65"/>
+      <c r="M51" s="65"/>
+      <c r="N51" s="65"/>
     </row>
     <row r="52" spans="1:15" ht="15" customHeight="1">
       <c r="A52" s="31" t="s">
@@ -1693,174 +1692,208 @@
       <c r="C52" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D52" s="67"/>
-      <c r="E52" s="67"/>
-      <c r="F52" s="67"/>
-      <c r="G52" s="67"/>
-      <c r="H52" s="67"/>
-      <c r="I52" s="67"/>
-      <c r="J52" s="67"/>
-      <c r="K52" s="68"/>
+      <c r="D52" s="55"/>
+      <c r="E52" s="55"/>
+      <c r="F52" s="55"/>
+      <c r="G52" s="55"/>
+      <c r="H52" s="55"/>
+      <c r="I52" s="55"/>
+      <c r="J52" s="55"/>
+      <c r="K52" s="56"/>
     </row>
     <row r="53" spans="1:15" ht="4.5" customHeight="1"/>
     <row r="54" spans="1:15">
-      <c r="A54" s="69" t="s">
+      <c r="A54" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="B54" s="69"/>
+      <c r="B54" s="54"/>
       <c r="C54" s="10"/>
-      <c r="D54" s="69" t="s">
+      <c r="D54" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="E54" s="69"/>
-      <c r="F54" s="69"/>
-      <c r="G54" s="69"/>
-      <c r="H54" s="69"/>
-      <c r="I54" s="69"/>
+      <c r="E54" s="54"/>
+      <c r="F54" s="54"/>
+      <c r="G54" s="54"/>
+      <c r="H54" s="54"/>
+      <c r="I54" s="54"/>
       <c r="J54" s="10"/>
-      <c r="K54" s="69" t="s">
+      <c r="K54" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="L54" s="69"/>
-      <c r="M54" s="69"/>
-      <c r="N54" s="69"/>
+      <c r="L54" s="54"/>
+      <c r="M54" s="54"/>
+      <c r="N54" s="54"/>
     </row>
     <row r="55" spans="1:15">
-      <c r="A55" s="69" t="s">
+      <c r="A55" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="B55" s="69"/>
+      <c r="B55" s="54"/>
       <c r="C55" s="10"/>
-      <c r="D55" s="69" t="s">
+      <c r="D55" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="E55" s="69"/>
-      <c r="F55" s="69" t="s">
+      <c r="E55" s="54"/>
+      <c r="F55" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="G55" s="69"/>
-      <c r="H55" s="69" t="s">
+      <c r="G55" s="54"/>
+      <c r="H55" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="I55" s="69"/>
+      <c r="I55" s="54"/>
       <c r="J55" s="25"/>
-      <c r="K55" s="69" t="s">
+      <c r="K55" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="L55" s="69"/>
-      <c r="M55" s="69" t="s">
+      <c r="L55" s="54"/>
+      <c r="M55" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="N55" s="69"/>
+      <c r="N55" s="54"/>
     </row>
     <row r="56" spans="1:15">
-      <c r="A56" s="69"/>
-      <c r="B56" s="69"/>
+      <c r="A56" s="54"/>
+      <c r="B56" s="54"/>
       <c r="C56" s="10"/>
-      <c r="D56" s="69"/>
-      <c r="E56" s="69"/>
-      <c r="F56" s="69"/>
-      <c r="G56" s="69"/>
-      <c r="H56" s="69"/>
-      <c r="I56" s="69"/>
+      <c r="D56" s="54"/>
+      <c r="E56" s="54"/>
+      <c r="F56" s="54"/>
+      <c r="G56" s="54"/>
+      <c r="H56" s="54"/>
+      <c r="I56" s="54"/>
       <c r="J56" s="10"/>
-      <c r="K56" s="69"/>
-      <c r="L56" s="69"/>
-      <c r="M56" s="69"/>
-      <c r="N56" s="69"/>
+      <c r="K56" s="54"/>
+      <c r="L56" s="54"/>
+      <c r="M56" s="54"/>
+      <c r="N56" s="54"/>
     </row>
     <row r="57" spans="1:15">
-      <c r="A57" s="69"/>
-      <c r="B57" s="69"/>
+      <c r="A57" s="54"/>
+      <c r="B57" s="54"/>
       <c r="C57" s="10"/>
-      <c r="D57" s="69"/>
-      <c r="E57" s="69"/>
-      <c r="F57" s="69"/>
-      <c r="G57" s="69"/>
-      <c r="H57" s="69"/>
-      <c r="I57" s="69"/>
+      <c r="D57" s="54"/>
+      <c r="E57" s="54"/>
+      <c r="F57" s="54"/>
+      <c r="G57" s="54"/>
+      <c r="H57" s="54"/>
+      <c r="I57" s="54"/>
       <c r="J57" s="10"/>
-      <c r="K57" s="69"/>
-      <c r="L57" s="69"/>
-      <c r="M57" s="69"/>
-      <c r="N57" s="69"/>
+      <c r="K57" s="54"/>
+      <c r="L57" s="54"/>
+      <c r="M57" s="54"/>
+      <c r="N57" s="54"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="69"/>
-      <c r="B58" s="69"/>
+      <c r="A58" s="54"/>
+      <c r="B58" s="54"/>
       <c r="C58" s="10"/>
-      <c r="D58" s="69"/>
-      <c r="E58" s="69"/>
-      <c r="F58" s="69"/>
-      <c r="G58" s="69"/>
-      <c r="H58" s="69"/>
-      <c r="I58" s="69"/>
+      <c r="D58" s="54"/>
+      <c r="E58" s="54"/>
+      <c r="F58" s="54"/>
+      <c r="G58" s="54"/>
+      <c r="H58" s="54"/>
+      <c r="I58" s="54"/>
       <c r="J58" s="10"/>
-      <c r="K58" s="69"/>
-      <c r="L58" s="69"/>
-      <c r="M58" s="69"/>
-      <c r="N58" s="69"/>
+      <c r="K58" s="54"/>
+      <c r="L58" s="54"/>
+      <c r="M58" s="54"/>
+      <c r="N58" s="54"/>
     </row>
     <row r="59" spans="1:15">
-      <c r="A59" s="69"/>
-      <c r="B59" s="69"/>
+      <c r="A59" s="54"/>
+      <c r="B59" s="54"/>
       <c r="C59" s="10"/>
-      <c r="D59" s="69"/>
-      <c r="E59" s="69"/>
-      <c r="F59" s="69"/>
-      <c r="G59" s="69"/>
-      <c r="H59" s="69"/>
-      <c r="I59" s="69"/>
+      <c r="D59" s="54"/>
+      <c r="E59" s="54"/>
+      <c r="F59" s="54"/>
+      <c r="G59" s="54"/>
+      <c r="H59" s="54"/>
+      <c r="I59" s="54"/>
       <c r="J59" s="10"/>
-      <c r="K59" s="69"/>
-      <c r="L59" s="69"/>
-      <c r="M59" s="69"/>
-      <c r="N59" s="69"/>
+      <c r="K59" s="54"/>
+      <c r="L59" s="54"/>
+      <c r="M59" s="54"/>
+      <c r="N59" s="54"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="69" t="s">
+      <c r="A60" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="69"/>
+      <c r="B60" s="54"/>
       <c r="C60" s="10"/>
-      <c r="D60" s="69" t="s">
+      <c r="D60" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="E60" s="69"/>
-      <c r="F60" s="69" t="s">
+      <c r="E60" s="54"/>
+      <c r="F60" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="G60" s="69"/>
-      <c r="H60" s="69" t="s">
+      <c r="G60" s="54"/>
+      <c r="H60" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="I60" s="69"/>
+      <c r="I60" s="54"/>
       <c r="J60" s="10"/>
-      <c r="K60" s="69" t="s">
+      <c r="K60" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="L60" s="69"/>
-      <c r="M60" s="69" t="s">
+      <c r="L60" s="54"/>
+      <c r="M60" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="N60" s="69"/>
+      <c r="N60" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="I7:N8"/>
-    <mergeCell ref="D12:K12"/>
-    <mergeCell ref="D11:K11"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="F15:G17"/>
-    <mergeCell ref="H15:K17"/>
-    <mergeCell ref="L15:N17"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="L18:N18"/>
-    <mergeCell ref="K22:N22"/>
-    <mergeCell ref="D19:N21"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:H38"/>
+    <mergeCell ref="L46:N46"/>
+    <mergeCell ref="L50:N50"/>
+    <mergeCell ref="L51:N51"/>
+    <mergeCell ref="D50:K50"/>
+    <mergeCell ref="D51:K51"/>
+    <mergeCell ref="C46:K47"/>
+    <mergeCell ref="A41:G44"/>
+    <mergeCell ref="H40:K40"/>
+    <mergeCell ref="H41:K44"/>
+    <mergeCell ref="L41:N44"/>
+    <mergeCell ref="L40:N40"/>
+    <mergeCell ref="A40:G40"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="L38:N38"/>
+    <mergeCell ref="E37:H37"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B26"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="D52:K52"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A56:B59"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="K54:N54"/>
+    <mergeCell ref="D54:I54"/>
+    <mergeCell ref="M55:N55"/>
+    <mergeCell ref="D56:E59"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="F56:G59"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="H56:I59"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="K56:L59"/>
+    <mergeCell ref="M56:N59"/>
+    <mergeCell ref="K60:L60"/>
+    <mergeCell ref="M60:N60"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="K55:L55"/>
     <mergeCell ref="J38:K38"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B15:E17"/>
@@ -1877,54 +1910,20 @@
     <mergeCell ref="K26:N26"/>
     <mergeCell ref="K27:N27"/>
     <mergeCell ref="K23:N24"/>
-    <mergeCell ref="M56:N59"/>
-    <mergeCell ref="K60:L60"/>
-    <mergeCell ref="M60:N60"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="D52:K52"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A56:B59"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="K54:N54"/>
-    <mergeCell ref="D54:I54"/>
-    <mergeCell ref="M55:N55"/>
-    <mergeCell ref="D56:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="F56:G59"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="H56:I59"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="K56:L59"/>
-    <mergeCell ref="E37:H37"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B26"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:H38"/>
-    <mergeCell ref="L46:N46"/>
-    <mergeCell ref="L50:N50"/>
-    <mergeCell ref="L51:N51"/>
-    <mergeCell ref="D50:K50"/>
-    <mergeCell ref="D51:K51"/>
-    <mergeCell ref="C46:K47"/>
-    <mergeCell ref="A41:G44"/>
-    <mergeCell ref="H40:K40"/>
-    <mergeCell ref="H41:K44"/>
-    <mergeCell ref="L41:N44"/>
-    <mergeCell ref="L40:N40"/>
-    <mergeCell ref="A40:G40"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="L38:N38"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="F15:G17"/>
+    <mergeCell ref="H15:K17"/>
+    <mergeCell ref="L15:N17"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="L18:N18"/>
+    <mergeCell ref="K22:N22"/>
+    <mergeCell ref="D19:N21"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="I7:N8"/>
+    <mergeCell ref="D12:K12"/>
+    <mergeCell ref="D11:K11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0" bottom="0" header="0" footer="0.3"/>

</xml_diff>

<commit_message>
hotfix-3.0.3 : revisi tanda terima dan invoice
</commit_message>
<xml_diff>
--- a/storage/template/tandaterima.xlsx
+++ b/storage/template/tandaterima.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\solidnew\storage\template\"/>
@@ -14,8 +14,11 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$N$60</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$30:$N$61</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -198,7 +201,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,6 +283,12 @@
       <color theme="1"/>
       <name val="Free 3 of 9 Extended"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -433,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -490,66 +499,73 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -618,9 +634,6 @@
     </xf>
     <xf numFmtId="3" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -637,6 +650,14 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" firstButton="1" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -729,7 +750,193 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>16</xdr:col>
+          <xdr:colOff>95250</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>18</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>104775</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1027" name="Option Button 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1027"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Print Tanda Terima</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>16</xdr:col>
+          <xdr:colOff>95250</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>95250</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>18</xdr:col>
+          <xdr:colOff>361950</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>114300</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1028" name="Option Button 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1028"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Print Invoice Verification</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="tandaterima (1)"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="printTandaTerima"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -994,11 +1201,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:O60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A3:T60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7:N8"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1012,61 +1220,93 @@
     <col min="11" max="14" width="7.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:15" ht="17.25">
+    <row r="3" spans="1:20">
+      <c r="P3" s="38"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="38"/>
+    </row>
+    <row r="4" spans="1:20" ht="17.25">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="15.75">
+      <c r="P4" s="38"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="39"/>
+      <c r="T4" s="38"/>
+    </row>
+    <row r="5" spans="1:20" ht="15.75">
       <c r="I5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="38" t="s">
+      <c r="K5" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
       <c r="O5" s="27"/>
-    </row>
-    <row r="6" spans="1:15" ht="15.75">
+      <c r="P5" s="38"/>
+      <c r="Q5" s="38"/>
+      <c r="R5" s="38"/>
+      <c r="S5" s="38"/>
+      <c r="T5" s="38"/>
+    </row>
+    <row r="6" spans="1:20" ht="15.75">
       <c r="I6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="39"/>
-    </row>
-    <row r="7" spans="1:15" ht="17.25">
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="39"/>
+      <c r="S6" s="39"/>
+      <c r="T6" s="38"/>
+    </row>
+    <row r="7" spans="1:20" ht="17.25">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="81"/>
-      <c r="J7" s="81"/>
-      <c r="K7" s="81"/>
-      <c r="L7" s="81"/>
-      <c r="M7" s="81"/>
-      <c r="N7" s="81"/>
-    </row>
-    <row r="8" spans="1:15" ht="17.25">
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="42"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="39"/>
+      <c r="R7" s="39"/>
+      <c r="S7" s="39"/>
+      <c r="T7" s="38"/>
+    </row>
+    <row r="8" spans="1:20" ht="17.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="81"/>
-      <c r="J8" s="81"/>
-      <c r="K8" s="81"/>
-      <c r="L8" s="81"/>
-      <c r="M8" s="81"/>
-      <c r="N8" s="81"/>
-    </row>
-    <row r="9" spans="1:15" ht="17.25">
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="42"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="38"/>
+      <c r="R8" s="38"/>
+      <c r="S8" s="38"/>
+      <c r="T8" s="38"/>
+    </row>
+    <row r="9" spans="1:20" ht="17.25">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -1076,53 +1316,53 @@
       <c r="J9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
-      <c r="N9" s="38"/>
-    </row>
-    <row r="10" spans="1:15" ht="16.5" customHeight="1">
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
+    </row>
+    <row r="10" spans="1:20" ht="16.5" customHeight="1">
       <c r="F10" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="17.25">
-      <c r="A11" s="38" t="s">
+    <row r="11" spans="1:20" ht="17.25">
+      <c r="A11" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="38"/>
+      <c r="B11" s="40"/>
       <c r="C11" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="60"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:15" ht="17.25">
-      <c r="A12" s="38" t="s">
+    <row r="12" spans="1:20" ht="17.25">
+      <c r="A12" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="38"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="40"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:15" ht="15" customHeight="1">
+    <row r="13" spans="1:20" ht="15" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1136,177 +1376,177 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:20">
       <c r="A14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41" t="s">
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41" t="s">
+      <c r="G14" s="43"/>
+      <c r="H14" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="41"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="41" t="s">
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="M14" s="41"/>
-      <c r="N14" s="41"/>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="A15" s="42">
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="44">
         <v>1</v>
       </c>
-      <c r="B15" s="42"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="42"/>
-      <c r="L15" s="42"/>
-      <c r="M15" s="42"/>
-      <c r="N15" s="42"/>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="A16" s="42"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="42"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="42"/>
-      <c r="N16" s="42"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="44"/>
+      <c r="M15" s="44"/>
+      <c r="N15" s="44"/>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="44"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="44"/>
+      <c r="M16" s="44"/>
+      <c r="N16" s="44"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="42"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="42"/>
-      <c r="N17" s="42"/>
+      <c r="A17" s="44"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="44"/>
+      <c r="L17" s="44"/>
+      <c r="M17" s="44"/>
+      <c r="N17" s="44"/>
     </row>
     <row r="18" spans="1:14" ht="17.25">
       <c r="A18" s="6"/>
-      <c r="B18" s="48"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="48"/>
-      <c r="L18" s="42"/>
-      <c r="M18" s="42"/>
-      <c r="N18" s="42"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="44"/>
+      <c r="M18" s="44"/>
+      <c r="N18" s="44"/>
     </row>
     <row r="19" spans="1:14" ht="6.75" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="45"/>
-      <c r="L19" s="45"/>
-      <c r="M19" s="45"/>
-      <c r="N19" s="45"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="46"/>
+      <c r="M19" s="46"/>
+      <c r="N19" s="46"/>
     </row>
     <row r="20" spans="1:14" ht="15.75">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="38"/>
+      <c r="B20" s="40"/>
       <c r="C20" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
-      <c r="K20" s="46"/>
-      <c r="L20" s="46"/>
-      <c r="M20" s="46"/>
-      <c r="N20" s="46"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="47"/>
     </row>
     <row r="21" spans="1:14" ht="6.75" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="46"/>
-      <c r="K21" s="46"/>
-      <c r="L21" s="46"/>
-      <c r="M21" s="46"/>
-      <c r="N21" s="46"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="47"/>
     </row>
     <row r="22" spans="1:14" ht="17.25">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43" t="s">
+      <c r="B22" s="51"/>
+      <c r="C22" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
       <c r="F22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="7" t="s">
         <v>17</v>
       </c>
       <c r="J22" s="1"/>
-      <c r="K22" s="44"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="44"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="45"/>
+      <c r="M22" s="45"/>
+      <c r="N22" s="45"/>
     </row>
     <row r="23" spans="1:14" ht="15.75">
-      <c r="A23" s="49"/>
-      <c r="B23" s="49"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
+      <c r="A23" s="50"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
       <c r="G23" s="7" t="s">
         <v>18</v>
       </c>
@@ -1314,28 +1554,28 @@
       <c r="J23" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K23" s="53"/>
-      <c r="L23" s="53"/>
-      <c r="M23" s="53"/>
-      <c r="N23" s="53"/>
+      <c r="K23" s="55"/>
+      <c r="L23" s="55"/>
+      <c r="M23" s="55"/>
+      <c r="N23" s="55"/>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A24" s="49"/>
-      <c r="B24" s="49"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="K24" s="53"/>
-      <c r="L24" s="53"/>
-      <c r="M24" s="53"/>
-      <c r="N24" s="53"/>
+      <c r="A24" s="50"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="K24" s="55"/>
+      <c r="L24" s="55"/>
+      <c r="M24" s="55"/>
+      <c r="N24" s="55"/>
     </row>
     <row r="25" spans="1:14" ht="15.75">
-      <c r="A25" s="49"/>
-      <c r="B25" s="49"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
       <c r="G25" s="7" t="s">
         <v>19</v>
       </c>
@@ -1343,17 +1583,17 @@
       <c r="J25" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K25" s="52"/>
-      <c r="L25" s="52"/>
-      <c r="M25" s="52"/>
-      <c r="N25" s="52"/>
+      <c r="K25" s="54"/>
+      <c r="L25" s="54"/>
+      <c r="M25" s="54"/>
+      <c r="N25" s="54"/>
     </row>
     <row r="26" spans="1:14" ht="15.75">
-      <c r="A26" s="49"/>
-      <c r="B26" s="49"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
+      <c r="A26" s="50"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
       <c r="G26" s="7" t="s">
         <v>20</v>
       </c>
@@ -1361,17 +1601,17 @@
       <c r="J26" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K26" s="52"/>
-      <c r="L26" s="52"/>
-      <c r="M26" s="52"/>
-      <c r="N26" s="52"/>
+      <c r="K26" s="54"/>
+      <c r="L26" s="54"/>
+      <c r="M26" s="54"/>
+      <c r="N26" s="54"/>
     </row>
     <row r="27" spans="1:14" ht="15.75">
-      <c r="A27" s="49"/>
-      <c r="B27" s="49"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
+      <c r="A27" s="50"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
       <c r="G27" s="7" t="s">
         <v>21</v>
       </c>
@@ -1379,10 +1619,10 @@
       <c r="J27" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K27" s="52"/>
-      <c r="L27" s="52"/>
-      <c r="M27" s="52"/>
-      <c r="N27" s="52"/>
+      <c r="K27" s="54"/>
+      <c r="L27" s="54"/>
+      <c r="M27" s="54"/>
+      <c r="N27" s="54"/>
     </row>
     <row r="29" spans="1:14" ht="40.5" customHeight="1"/>
     <row r="31" spans="1:14">
@@ -1439,188 +1679,188 @@
       <c r="J34" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K34" s="51"/>
-      <c r="L34" s="51"/>
-      <c r="M34" s="51"/>
-      <c r="N34" s="51"/>
+      <c r="K34" s="53"/>
+      <c r="L34" s="53"/>
+      <c r="M34" s="53"/>
+      <c r="N34" s="53"/>
     </row>
     <row r="35" spans="1:14">
       <c r="A35" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D35" s="12"/>
-      <c r="E35" s="50" t="s">
+      <c r="E35" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="50"/>
+      <c r="F35" s="52"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="52"/>
       <c r="I35" s="9" t="s">
         <v>25</v>
       </c>
       <c r="J35" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K35" s="51"/>
-      <c r="L35" s="51"/>
-      <c r="M35" s="51"/>
-      <c r="N35" s="51"/>
+      <c r="K35" s="53"/>
+      <c r="L35" s="53"/>
+      <c r="M35" s="53"/>
+      <c r="N35" s="53"/>
     </row>
     <row r="36" spans="1:14">
-      <c r="E36" s="50" t="s">
+      <c r="E36" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="F36" s="50"/>
-      <c r="G36" s="50"/>
-      <c r="H36" s="50"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="52"/>
     </row>
     <row r="37" spans="1:14" ht="18" customHeight="1">
       <c r="D37" s="26"/>
-      <c r="E37" s="57"/>
-      <c r="F37" s="57"/>
-      <c r="G37" s="57"/>
-      <c r="H37" s="57"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
+      <c r="G37" s="59"/>
+      <c r="H37" s="59"/>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="58" t="s">
+      <c r="A38" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="58"/>
-      <c r="C38" s="59"/>
-      <c r="D38" s="60"/>
-      <c r="E38" s="60"/>
-      <c r="F38" s="60"/>
-      <c r="G38" s="60"/>
-      <c r="H38" s="61"/>
+      <c r="B38" s="61"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="63"/>
+      <c r="E38" s="63"/>
+      <c r="F38" s="63"/>
+      <c r="G38" s="63"/>
+      <c r="H38" s="64"/>
       <c r="I38" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="J38" s="47"/>
-      <c r="K38" s="47"/>
-      <c r="L38" s="79"/>
-      <c r="M38" s="79"/>
-      <c r="N38" s="80"/>
+      <c r="J38" s="48"/>
+      <c r="K38" s="48"/>
+      <c r="L38" s="82"/>
+      <c r="M38" s="82"/>
+      <c r="N38" s="83"/>
     </row>
     <row r="39" spans="1:14" ht="3.75" customHeight="1">
       <c r="J39" s="19"/>
     </row>
     <row r="40" spans="1:14">
-      <c r="A40" s="75" t="s">
+      <c r="A40" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="75"/>
-      <c r="C40" s="75"/>
-      <c r="D40" s="75"/>
-      <c r="E40" s="75"/>
-      <c r="F40" s="75"/>
-      <c r="G40" s="75"/>
-      <c r="H40" s="75" t="s">
+      <c r="B40" s="78"/>
+      <c r="C40" s="78"/>
+      <c r="D40" s="78"/>
+      <c r="E40" s="78"/>
+      <c r="F40" s="78"/>
+      <c r="G40" s="78"/>
+      <c r="H40" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="I40" s="75"/>
-      <c r="J40" s="75"/>
-      <c r="K40" s="75"/>
-      <c r="L40" s="75" t="s">
+      <c r="I40" s="78"/>
+      <c r="J40" s="78"/>
+      <c r="K40" s="78"/>
+      <c r="L40" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="M40" s="75"/>
-      <c r="N40" s="75"/>
+      <c r="M40" s="78"/>
+      <c r="N40" s="78"/>
     </row>
     <row r="41" spans="1:14">
-      <c r="A41" s="74"/>
-      <c r="B41" s="74"/>
-      <c r="C41" s="74"/>
-      <c r="D41" s="74"/>
-      <c r="E41" s="74"/>
-      <c r="F41" s="74"/>
-      <c r="G41" s="74"/>
-      <c r="H41" s="74"/>
-      <c r="I41" s="74"/>
-      <c r="J41" s="74"/>
-      <c r="K41" s="74"/>
-      <c r="L41" s="76"/>
-      <c r="M41" s="76"/>
-      <c r="N41" s="76"/>
+      <c r="A41" s="77"/>
+      <c r="B41" s="77"/>
+      <c r="C41" s="77"/>
+      <c r="D41" s="77"/>
+      <c r="E41" s="77"/>
+      <c r="F41" s="77"/>
+      <c r="G41" s="77"/>
+      <c r="H41" s="77"/>
+      <c r="I41" s="77"/>
+      <c r="J41" s="77"/>
+      <c r="K41" s="77"/>
+      <c r="L41" s="79"/>
+      <c r="M41" s="79"/>
+      <c r="N41" s="79"/>
     </row>
     <row r="42" spans="1:14">
-      <c r="A42" s="74"/>
-      <c r="B42" s="74"/>
-      <c r="C42" s="74"/>
-      <c r="D42" s="74"/>
-      <c r="E42" s="74"/>
-      <c r="F42" s="74"/>
-      <c r="G42" s="74"/>
-      <c r="H42" s="74"/>
-      <c r="I42" s="74"/>
-      <c r="J42" s="74"/>
-      <c r="K42" s="74"/>
-      <c r="L42" s="76"/>
-      <c r="M42" s="76"/>
-      <c r="N42" s="76"/>
+      <c r="A42" s="77"/>
+      <c r="B42" s="77"/>
+      <c r="C42" s="77"/>
+      <c r="D42" s="77"/>
+      <c r="E42" s="77"/>
+      <c r="F42" s="77"/>
+      <c r="G42" s="77"/>
+      <c r="H42" s="77"/>
+      <c r="I42" s="77"/>
+      <c r="J42" s="77"/>
+      <c r="K42" s="77"/>
+      <c r="L42" s="79"/>
+      <c r="M42" s="79"/>
+      <c r="N42" s="79"/>
     </row>
     <row r="43" spans="1:14">
-      <c r="A43" s="74"/>
-      <c r="B43" s="74"/>
-      <c r="C43" s="74"/>
-      <c r="D43" s="74"/>
-      <c r="E43" s="74"/>
-      <c r="F43" s="74"/>
-      <c r="G43" s="74"/>
-      <c r="H43" s="74"/>
-      <c r="I43" s="74"/>
-      <c r="J43" s="74"/>
-      <c r="K43" s="74"/>
-      <c r="L43" s="76"/>
-      <c r="M43" s="76"/>
-      <c r="N43" s="76"/>
+      <c r="A43" s="77"/>
+      <c r="B43" s="77"/>
+      <c r="C43" s="77"/>
+      <c r="D43" s="77"/>
+      <c r="E43" s="77"/>
+      <c r="F43" s="77"/>
+      <c r="G43" s="77"/>
+      <c r="H43" s="77"/>
+      <c r="I43" s="77"/>
+      <c r="J43" s="77"/>
+      <c r="K43" s="77"/>
+      <c r="L43" s="79"/>
+      <c r="M43" s="79"/>
+      <c r="N43" s="79"/>
     </row>
     <row r="44" spans="1:14">
-      <c r="A44" s="74"/>
-      <c r="B44" s="74"/>
-      <c r="C44" s="74"/>
-      <c r="D44" s="74"/>
-      <c r="E44" s="74"/>
-      <c r="F44" s="74"/>
-      <c r="G44" s="74"/>
-      <c r="H44" s="74"/>
-      <c r="I44" s="74"/>
-      <c r="J44" s="74"/>
-      <c r="K44" s="74"/>
-      <c r="L44" s="76"/>
-      <c r="M44" s="76"/>
-      <c r="N44" s="76"/>
+      <c r="A44" s="77"/>
+      <c r="B44" s="77"/>
+      <c r="C44" s="77"/>
+      <c r="D44" s="77"/>
+      <c r="E44" s="77"/>
+      <c r="F44" s="77"/>
+      <c r="G44" s="77"/>
+      <c r="H44" s="77"/>
+      <c r="I44" s="77"/>
+      <c r="J44" s="77"/>
+      <c r="K44" s="77"/>
+      <c r="L44" s="79"/>
+      <c r="M44" s="79"/>
+      <c r="N44" s="79"/>
     </row>
     <row r="45" spans="1:14" ht="3.75" customHeight="1"/>
     <row r="46" spans="1:14">
-      <c r="A46" s="77" t="s">
+      <c r="A46" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="78"/>
-      <c r="C46" s="70"/>
-      <c r="D46" s="70"/>
-      <c r="E46" s="70"/>
-      <c r="F46" s="70"/>
-      <c r="G46" s="70"/>
-      <c r="H46" s="70"/>
-      <c r="I46" s="70"/>
-      <c r="J46" s="70"/>
-      <c r="K46" s="71"/>
-      <c r="L46" s="62"/>
-      <c r="M46" s="63"/>
-      <c r="N46" s="64"/>
+      <c r="B46" s="81"/>
+      <c r="C46" s="73"/>
+      <c r="D46" s="73"/>
+      <c r="E46" s="73"/>
+      <c r="F46" s="73"/>
+      <c r="G46" s="73"/>
+      <c r="H46" s="73"/>
+      <c r="I46" s="73"/>
+      <c r="J46" s="73"/>
+      <c r="K46" s="74"/>
+      <c r="L46" s="65"/>
+      <c r="M46" s="66"/>
+      <c r="N46" s="67"/>
     </row>
     <row r="47" spans="1:14" ht="15" customHeight="1">
       <c r="A47" s="14"/>
       <c r="B47" s="15"/>
-      <c r="C47" s="72"/>
-      <c r="D47" s="72"/>
-      <c r="E47" s="72"/>
-      <c r="F47" s="72"/>
-      <c r="G47" s="72"/>
-      <c r="H47" s="72"/>
-      <c r="I47" s="72"/>
-      <c r="J47" s="72"/>
-      <c r="K47" s="73"/>
+      <c r="C47" s="75"/>
+      <c r="D47" s="75"/>
+      <c r="E47" s="75"/>
+      <c r="F47" s="75"/>
+      <c r="G47" s="75"/>
+      <c r="H47" s="75"/>
+      <c r="I47" s="75"/>
+      <c r="J47" s="75"/>
+      <c r="K47" s="76"/>
       <c r="L47" s="14"/>
       <c r="M47" s="15"/>
       <c r="N47" s="16"/>
@@ -1649,19 +1889,19 @@
       <c r="C50" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D50" s="66"/>
-      <c r="E50" s="66"/>
-      <c r="F50" s="66"/>
-      <c r="G50" s="66"/>
-      <c r="H50" s="66"/>
-      <c r="I50" s="66"/>
-      <c r="J50" s="66"/>
-      <c r="K50" s="67"/>
-      <c r="L50" s="65" t="s">
+      <c r="D50" s="69"/>
+      <c r="E50" s="69"/>
+      <c r="F50" s="69"/>
+      <c r="G50" s="69"/>
+      <c r="H50" s="69"/>
+      <c r="I50" s="69"/>
+      <c r="J50" s="69"/>
+      <c r="K50" s="70"/>
+      <c r="L50" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="M50" s="65"/>
-      <c r="N50" s="65"/>
+      <c r="M50" s="68"/>
+      <c r="N50" s="68"/>
       <c r="O50" s="11"/>
     </row>
     <row r="51" spans="1:15">
@@ -1672,17 +1912,17 @@
       <c r="C51" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D51" s="68"/>
-      <c r="E51" s="68"/>
-      <c r="F51" s="68"/>
-      <c r="G51" s="68"/>
-      <c r="H51" s="68"/>
-      <c r="I51" s="68"/>
-      <c r="J51" s="68"/>
-      <c r="K51" s="69"/>
-      <c r="L51" s="65"/>
-      <c r="M51" s="65"/>
-      <c r="N51" s="65"/>
+      <c r="D51" s="71"/>
+      <c r="E51" s="71"/>
+      <c r="F51" s="71"/>
+      <c r="G51" s="71"/>
+      <c r="H51" s="71"/>
+      <c r="I51" s="71"/>
+      <c r="J51" s="71"/>
+      <c r="K51" s="72"/>
+      <c r="L51" s="68"/>
+      <c r="M51" s="68"/>
+      <c r="N51" s="68"/>
     </row>
     <row r="52" spans="1:15" ht="15" customHeight="1">
       <c r="A52" s="31" t="s">
@@ -1692,160 +1932,160 @@
       <c r="C52" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D52" s="55"/>
-      <c r="E52" s="55"/>
-      <c r="F52" s="55"/>
-      <c r="G52" s="55"/>
-      <c r="H52" s="55"/>
-      <c r="I52" s="55"/>
-      <c r="J52" s="55"/>
-      <c r="K52" s="56"/>
+      <c r="D52" s="57"/>
+      <c r="E52" s="57"/>
+      <c r="F52" s="57"/>
+      <c r="G52" s="57"/>
+      <c r="H52" s="57"/>
+      <c r="I52" s="57"/>
+      <c r="J52" s="57"/>
+      <c r="K52" s="58"/>
     </row>
     <row r="53" spans="1:15" ht="4.5" customHeight="1"/>
     <row r="54" spans="1:15">
-      <c r="A54" s="54" t="s">
+      <c r="A54" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="B54" s="54"/>
+      <c r="B54" s="56"/>
       <c r="C54" s="10"/>
-      <c r="D54" s="54" t="s">
+      <c r="D54" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="E54" s="54"/>
-      <c r="F54" s="54"/>
-      <c r="G54" s="54"/>
-      <c r="H54" s="54"/>
-      <c r="I54" s="54"/>
+      <c r="E54" s="56"/>
+      <c r="F54" s="56"/>
+      <c r="G54" s="56"/>
+      <c r="H54" s="56"/>
+      <c r="I54" s="56"/>
       <c r="J54" s="10"/>
-      <c r="K54" s="54" t="s">
+      <c r="K54" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="L54" s="54"/>
-      <c r="M54" s="54"/>
-      <c r="N54" s="54"/>
+      <c r="L54" s="56"/>
+      <c r="M54" s="56"/>
+      <c r="N54" s="56"/>
     </row>
     <row r="55" spans="1:15">
-      <c r="A55" s="54" t="s">
+      <c r="A55" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="B55" s="54"/>
+      <c r="B55" s="56"/>
       <c r="C55" s="10"/>
-      <c r="D55" s="54" t="s">
+      <c r="D55" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="E55" s="54"/>
-      <c r="F55" s="54" t="s">
+      <c r="E55" s="56"/>
+      <c r="F55" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="G55" s="54"/>
-      <c r="H55" s="54" t="s">
+      <c r="G55" s="56"/>
+      <c r="H55" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="I55" s="54"/>
+      <c r="I55" s="56"/>
       <c r="J55" s="25"/>
-      <c r="K55" s="54" t="s">
+      <c r="K55" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="L55" s="54"/>
-      <c r="M55" s="54" t="s">
+      <c r="L55" s="56"/>
+      <c r="M55" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="N55" s="54"/>
+      <c r="N55" s="56"/>
     </row>
     <row r="56" spans="1:15">
-      <c r="A56" s="54"/>
-      <c r="B56" s="54"/>
+      <c r="A56" s="56"/>
+      <c r="B56" s="56"/>
       <c r="C56" s="10"/>
-      <c r="D56" s="54"/>
-      <c r="E56" s="54"/>
-      <c r="F56" s="54"/>
-      <c r="G56" s="54"/>
-      <c r="H56" s="54"/>
-      <c r="I56" s="54"/>
+      <c r="D56" s="56"/>
+      <c r="E56" s="56"/>
+      <c r="F56" s="56"/>
+      <c r="G56" s="56"/>
+      <c r="H56" s="56"/>
+      <c r="I56" s="56"/>
       <c r="J56" s="10"/>
-      <c r="K56" s="54"/>
-      <c r="L56" s="54"/>
-      <c r="M56" s="54"/>
-      <c r="N56" s="54"/>
+      <c r="K56" s="56"/>
+      <c r="L56" s="56"/>
+      <c r="M56" s="56"/>
+      <c r="N56" s="56"/>
     </row>
     <row r="57" spans="1:15">
-      <c r="A57" s="54"/>
-      <c r="B57" s="54"/>
+      <c r="A57" s="56"/>
+      <c r="B57" s="56"/>
       <c r="C57" s="10"/>
-      <c r="D57" s="54"/>
-      <c r="E57" s="54"/>
-      <c r="F57" s="54"/>
-      <c r="G57" s="54"/>
-      <c r="H57" s="54"/>
-      <c r="I57" s="54"/>
+      <c r="D57" s="56"/>
+      <c r="E57" s="56"/>
+      <c r="F57" s="56"/>
+      <c r="G57" s="56"/>
+      <c r="H57" s="56"/>
+      <c r="I57" s="56"/>
       <c r="J57" s="10"/>
-      <c r="K57" s="54"/>
-      <c r="L57" s="54"/>
-      <c r="M57" s="54"/>
-      <c r="N57" s="54"/>
+      <c r="K57" s="56"/>
+      <c r="L57" s="56"/>
+      <c r="M57" s="56"/>
+      <c r="N57" s="56"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="54"/>
-      <c r="B58" s="54"/>
+      <c r="A58" s="56"/>
+      <c r="B58" s="56"/>
       <c r="C58" s="10"/>
-      <c r="D58" s="54"/>
-      <c r="E58" s="54"/>
-      <c r="F58" s="54"/>
-      <c r="G58" s="54"/>
-      <c r="H58" s="54"/>
-      <c r="I58" s="54"/>
+      <c r="D58" s="56"/>
+      <c r="E58" s="56"/>
+      <c r="F58" s="56"/>
+      <c r="G58" s="56"/>
+      <c r="H58" s="56"/>
+      <c r="I58" s="56"/>
       <c r="J58" s="10"/>
-      <c r="K58" s="54"/>
-      <c r="L58" s="54"/>
-      <c r="M58" s="54"/>
-      <c r="N58" s="54"/>
+      <c r="K58" s="56"/>
+      <c r="L58" s="56"/>
+      <c r="M58" s="56"/>
+      <c r="N58" s="56"/>
     </row>
     <row r="59" spans="1:15">
-      <c r="A59" s="54"/>
-      <c r="B59" s="54"/>
+      <c r="A59" s="56"/>
+      <c r="B59" s="56"/>
       <c r="C59" s="10"/>
-      <c r="D59" s="54"/>
-      <c r="E59" s="54"/>
-      <c r="F59" s="54"/>
-      <c r="G59" s="54"/>
-      <c r="H59" s="54"/>
-      <c r="I59" s="54"/>
+      <c r="D59" s="56"/>
+      <c r="E59" s="56"/>
+      <c r="F59" s="56"/>
+      <c r="G59" s="56"/>
+      <c r="H59" s="56"/>
+      <c r="I59" s="56"/>
       <c r="J59" s="10"/>
-      <c r="K59" s="54"/>
-      <c r="L59" s="54"/>
-      <c r="M59" s="54"/>
-      <c r="N59" s="54"/>
+      <c r="K59" s="56"/>
+      <c r="L59" s="56"/>
+      <c r="M59" s="56"/>
+      <c r="N59" s="56"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="54" t="s">
+      <c r="A60" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="54"/>
+      <c r="B60" s="56"/>
       <c r="C60" s="10"/>
-      <c r="D60" s="54" t="s">
+      <c r="D60" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="E60" s="54"/>
-      <c r="F60" s="54" t="s">
+      <c r="E60" s="56"/>
+      <c r="F60" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="G60" s="54"/>
-      <c r="H60" s="54" t="s">
+      <c r="G60" s="56"/>
+      <c r="H60" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="I60" s="54"/>
+      <c r="I60" s="56"/>
       <c r="J60" s="10"/>
-      <c r="K60" s="54" t="s">
+      <c r="K60" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="L60" s="54"/>
-      <c r="M60" s="54" t="s">
+      <c r="L60" s="56"/>
+      <c r="M60" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="N60" s="54"/>
+      <c r="N60" s="56"/>
     </row>
   </sheetData>
-  <mergeCells count="78">
+  <mergeCells count="80">
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:H38"/>
     <mergeCell ref="L46:N46"/>
@@ -1862,7 +2102,11 @@
     <mergeCell ref="A40:G40"/>
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="L38:N38"/>
-    <mergeCell ref="E37:H37"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="D12:K12"/>
+    <mergeCell ref="D11:K11"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
@@ -1870,8 +2114,6 @@
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A23:B26"/>
     <mergeCell ref="A20:B20"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:K18"/>
     <mergeCell ref="D52:K52"/>
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="A55:B55"/>
@@ -1894,12 +2136,11 @@
     <mergeCell ref="H55:I55"/>
     <mergeCell ref="F55:G55"/>
     <mergeCell ref="K55:L55"/>
+    <mergeCell ref="L18:N18"/>
+    <mergeCell ref="K22:N22"/>
+    <mergeCell ref="D19:N21"/>
     <mergeCell ref="J38:K38"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E17"/>
     <mergeCell ref="B18:E18"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:K14"/>
     <mergeCell ref="C23:E26"/>
     <mergeCell ref="C27:E27"/>
     <mergeCell ref="E35:H35"/>
@@ -1910,24 +2151,76 @@
     <mergeCell ref="K26:N26"/>
     <mergeCell ref="K27:N27"/>
     <mergeCell ref="K23:N24"/>
+    <mergeCell ref="E37:H37"/>
     <mergeCell ref="L14:N14"/>
     <mergeCell ref="F15:G17"/>
     <mergeCell ref="H15:K17"/>
     <mergeCell ref="L15:N17"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="L18:N18"/>
-    <mergeCell ref="K22:N22"/>
-    <mergeCell ref="D19:N21"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E17"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="Q3:S4"/>
+    <mergeCell ref="Q6:S7"/>
     <mergeCell ref="K5:N5"/>
     <mergeCell ref="K6:N6"/>
     <mergeCell ref="K9:N9"/>
     <mergeCell ref="I7:N8"/>
-    <mergeCell ref="D12:K12"/>
-    <mergeCell ref="D11:K11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0" bottom="0" header="0" footer="0.3"/>
   <pageSetup paperSize="9" scale="92" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1027" r:id="rId4" name="Option Button 3">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" macro="[1]!printTandaTerima">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>16</xdr:col>
+                    <xdr:colOff>95250</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>76200</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>18</xdr:col>
+                    <xdr:colOff>419100</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>104775</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1028" r:id="rId5" name="Option Button 4">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" macro="[0]!printInvoiceVoucherVerification">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>16</xdr:col>
+                    <xdr:colOff>95250</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>95250</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>18</xdr:col>
+                    <xdr:colOff>361950</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>114300</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
hotfix-1.0.9 : template solid
</commit_message>
<xml_diff>
--- a/storage/template/tandaterima.xlsx
+++ b/storage/template/tandaterima.xlsx
@@ -442,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -500,140 +500,143 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1205,8 +1208,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A3:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51:K51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1222,9 +1225,9 @@
   <sheetData>
     <row r="3" spans="1:20">
       <c r="P3" s="38"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
+      <c r="Q3" s="79"/>
+      <c r="R3" s="79"/>
+      <c r="S3" s="79"/>
       <c r="T3" s="38"/>
     </row>
     <row r="4" spans="1:20" ht="17.25">
@@ -1232,9 +1235,9 @@
         <v>0</v>
       </c>
       <c r="P4" s="38"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="39"/>
+      <c r="Q4" s="79"/>
+      <c r="R4" s="79"/>
+      <c r="S4" s="79"/>
       <c r="T4" s="38"/>
     </row>
     <row r="5" spans="1:20" ht="15.75">
@@ -1244,12 +1247,12 @@
       <c r="J5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="40" t="s">
+      <c r="K5" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="64"/>
+      <c r="N5" s="64"/>
       <c r="O5" s="27"/>
       <c r="P5" s="38"/>
       <c r="Q5" s="38"/>
@@ -1264,42 +1267,42 @@
       <c r="J6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="41"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="80"/>
+      <c r="M6" s="80"/>
+      <c r="N6" s="80"/>
       <c r="P6" s="38"/>
-      <c r="Q6" s="39"/>
-      <c r="R6" s="39"/>
-      <c r="S6" s="39"/>
+      <c r="Q6" s="79"/>
+      <c r="R6" s="79"/>
+      <c r="S6" s="79"/>
       <c r="T6" s="38"/>
     </row>
     <row r="7" spans="1:20" ht="17.25">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="42"/>
-      <c r="N7" s="42"/>
+      <c r="I7" s="81"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="81"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="81"/>
+      <c r="N7" s="81"/>
       <c r="P7" s="38"/>
-      <c r="Q7" s="39"/>
-      <c r="R7" s="39"/>
-      <c r="S7" s="39"/>
+      <c r="Q7" s="79"/>
+      <c r="R7" s="79"/>
+      <c r="S7" s="79"/>
       <c r="T7" s="38"/>
     </row>
     <row r="8" spans="1:20" ht="17.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="42"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="81"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="81"/>
+      <c r="N8" s="81"/>
       <c r="P8" s="38"/>
       <c r="Q8" s="38"/>
       <c r="R8" s="38"/>
@@ -1316,10 +1319,10 @@
       <c r="J9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="40"/>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40"/>
+      <c r="K9" s="64"/>
+      <c r="L9" s="64"/>
+      <c r="M9" s="64"/>
+      <c r="N9" s="64"/>
     </row>
     <row r="10" spans="1:20" ht="16.5" customHeight="1">
       <c r="F10" s="5" t="s">
@@ -1327,39 +1330,39 @@
       </c>
     </row>
     <row r="11" spans="1:20" ht="17.25">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="64" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="40"/>
+      <c r="B11" s="64"/>
       <c r="C11" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="60"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="62"/>
+      <c r="K11" s="62"/>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:20" ht="17.25">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="40"/>
+      <c r="B12" s="64"/>
       <c r="C12" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="60"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="62"/>
+      <c r="K12" s="62"/>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:20" ht="15" customHeight="1">
@@ -1380,173 +1383,173 @@
       <c r="A14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43" t="s">
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43" t="s">
+      <c r="G14" s="78"/>
+      <c r="H14" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="43"/>
-      <c r="L14" s="43" t="s">
+      <c r="I14" s="78"/>
+      <c r="J14" s="78"/>
+      <c r="K14" s="78"/>
+      <c r="L14" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="M14" s="43"/>
-      <c r="N14" s="43"/>
+      <c r="M14" s="78"/>
+      <c r="N14" s="78"/>
     </row>
     <row r="15" spans="1:20">
-      <c r="A15" s="44">
+      <c r="A15" s="63">
         <v>1</v>
       </c>
-      <c r="B15" s="44"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="44"/>
-      <c r="L15" s="44"/>
-      <c r="M15" s="44"/>
-      <c r="N15" s="44"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="63"/>
+      <c r="M15" s="63"/>
+      <c r="N15" s="63"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="44"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="44"/>
-      <c r="K16" s="44"/>
-      <c r="L16" s="44"/>
-      <c r="M16" s="44"/>
-      <c r="N16" s="44"/>
+      <c r="A16" s="63"/>
+      <c r="B16" s="63"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="63"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="63"/>
+      <c r="H16" s="63"/>
+      <c r="I16" s="63"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="63"/>
+      <c r="L16" s="63"/>
+      <c r="M16" s="63"/>
+      <c r="N16" s="63"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="44"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="44"/>
-      <c r="K17" s="44"/>
-      <c r="L17" s="44"/>
-      <c r="M17" s="44"/>
-      <c r="N17" s="44"/>
+      <c r="A17" s="63"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="63"/>
+      <c r="L17" s="63"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="63"/>
     </row>
     <row r="18" spans="1:14" ht="17.25">
       <c r="A18" s="6"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
-      <c r="K18" s="49"/>
-      <c r="L18" s="44"/>
-      <c r="M18" s="44"/>
-      <c r="N18" s="44"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="63"/>
+      <c r="M18" s="63"/>
+      <c r="N18" s="63"/>
     </row>
     <row r="19" spans="1:14" ht="6.75" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="46"/>
-      <c r="K19" s="46"/>
-      <c r="L19" s="46"/>
-      <c r="M19" s="46"/>
-      <c r="N19" s="46"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="70"/>
+      <c r="H19" s="70"/>
+      <c r="I19" s="70"/>
+      <c r="J19" s="70"/>
+      <c r="K19" s="70"/>
+      <c r="L19" s="70"/>
+      <c r="M19" s="70"/>
+      <c r="N19" s="70"/>
     </row>
     <row r="20" spans="1:14" ht="15.75">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="40"/>
+      <c r="B20" s="64"/>
       <c r="C20" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="47"/>
-      <c r="I20" s="47"/>
-      <c r="J20" s="47"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="47"/>
-      <c r="N20" s="47"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="71"/>
+      <c r="J20" s="71"/>
+      <c r="K20" s="71"/>
+      <c r="L20" s="71"/>
+      <c r="M20" s="71"/>
+      <c r="N20" s="71"/>
     </row>
     <row r="21" spans="1:14" ht="6.75" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="47"/>
-      <c r="N21" s="47"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="71"/>
+      <c r="J21" s="71"/>
+      <c r="K21" s="71"/>
+      <c r="L21" s="71"/>
+      <c r="M21" s="71"/>
+      <c r="N21" s="71"/>
     </row>
     <row r="22" spans="1:14" ht="17.25">
-      <c r="A22" s="51" t="s">
+      <c r="A22" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51" t="s">
+      <c r="B22" s="61"/>
+      <c r="C22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="51"/>
-      <c r="E22" s="51"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
       <c r="F22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="7" t="s">
         <v>17</v>
       </c>
       <c r="J22" s="1"/>
-      <c r="K22" s="45"/>
-      <c r="L22" s="45"/>
-      <c r="M22" s="45"/>
-      <c r="N22" s="45"/>
+      <c r="K22" s="69"/>
+      <c r="L22" s="69"/>
+      <c r="M22" s="69"/>
+      <c r="N22" s="69"/>
     </row>
     <row r="23" spans="1:14" ht="15.75">
-      <c r="A23" s="50"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
+      <c r="A23" s="65"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
       <c r="G23" s="7" t="s">
         <v>18</v>
       </c>
@@ -1554,28 +1557,28 @@
       <c r="J23" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K23" s="55"/>
-      <c r="L23" s="55"/>
-      <c r="M23" s="55"/>
-      <c r="N23" s="55"/>
+      <c r="K23" s="76"/>
+      <c r="L23" s="76"/>
+      <c r="M23" s="76"/>
+      <c r="N23" s="76"/>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A24" s="50"/>
-      <c r="B24" s="50"/>
-      <c r="C24" s="50"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50"/>
-      <c r="K24" s="55"/>
-      <c r="L24" s="55"/>
-      <c r="M24" s="55"/>
-      <c r="N24" s="55"/>
+      <c r="A24" s="65"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="K24" s="76"/>
+      <c r="L24" s="76"/>
+      <c r="M24" s="76"/>
+      <c r="N24" s="76"/>
     </row>
     <row r="25" spans="1:14" ht="15.75">
-      <c r="A25" s="50"/>
-      <c r="B25" s="50"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
+      <c r="A25" s="65"/>
+      <c r="B25" s="65"/>
+      <c r="C25" s="65"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
       <c r="G25" s="7" t="s">
         <v>19</v>
       </c>
@@ -1583,17 +1586,17 @@
       <c r="J25" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K25" s="54"/>
-      <c r="L25" s="54"/>
-      <c r="M25" s="54"/>
-      <c r="N25" s="54"/>
+      <c r="K25" s="82"/>
+      <c r="L25" s="82"/>
+      <c r="M25" s="82"/>
+      <c r="N25" s="82"/>
     </row>
     <row r="26" spans="1:14" ht="15.75">
-      <c r="A26" s="50"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
+      <c r="A26" s="65"/>
+      <c r="B26" s="65"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="65"/>
       <c r="G26" s="7" t="s">
         <v>20</v>
       </c>
@@ -1601,17 +1604,17 @@
       <c r="J26" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K26" s="54"/>
-      <c r="L26" s="54"/>
-      <c r="M26" s="54"/>
-      <c r="N26" s="54"/>
+      <c r="K26" s="75"/>
+      <c r="L26" s="75"/>
+      <c r="M26" s="75"/>
+      <c r="N26" s="75"/>
     </row>
     <row r="27" spans="1:14" ht="15.75">
-      <c r="A27" s="50"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="51"/>
+      <c r="A27" s="65"/>
+      <c r="B27" s="65"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
       <c r="G27" s="7" t="s">
         <v>21</v>
       </c>
@@ -1619,10 +1622,10 @@
       <c r="J27" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K27" s="54"/>
-      <c r="L27" s="54"/>
-      <c r="M27" s="54"/>
-      <c r="N27" s="54"/>
+      <c r="K27" s="75"/>
+      <c r="L27" s="75"/>
+      <c r="M27" s="75"/>
+      <c r="N27" s="75"/>
     </row>
     <row r="29" spans="1:14" ht="40.5" customHeight="1"/>
     <row r="31" spans="1:14">
@@ -1679,188 +1682,188 @@
       <c r="J34" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K34" s="53"/>
-      <c r="L34" s="53"/>
-      <c r="M34" s="53"/>
-      <c r="N34" s="53"/>
+      <c r="K34" s="74"/>
+      <c r="L34" s="74"/>
+      <c r="M34" s="74"/>
+      <c r="N34" s="74"/>
     </row>
     <row r="35" spans="1:14">
       <c r="A35" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D35" s="12"/>
-      <c r="E35" s="52" t="s">
+      <c r="E35" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="F35" s="52"/>
-      <c r="G35" s="52"/>
-      <c r="H35" s="52"/>
+      <c r="F35" s="73"/>
+      <c r="G35" s="73"/>
+      <c r="H35" s="73"/>
       <c r="I35" s="9" t="s">
         <v>25</v>
       </c>
       <c r="J35" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K35" s="53"/>
-      <c r="L35" s="53"/>
-      <c r="M35" s="53"/>
-      <c r="N35" s="53"/>
+      <c r="K35" s="74"/>
+      <c r="L35" s="74"/>
+      <c r="M35" s="74"/>
+      <c r="N35" s="74"/>
     </row>
     <row r="36" spans="1:14">
-      <c r="E36" s="52" t="s">
+      <c r="E36" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="F36" s="52"/>
-      <c r="G36" s="52"/>
-      <c r="H36" s="52"/>
+      <c r="F36" s="73"/>
+      <c r="G36" s="73"/>
+      <c r="H36" s="73"/>
     </row>
     <row r="37" spans="1:14" ht="18" customHeight="1">
       <c r="D37" s="26"/>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
-      <c r="G37" s="59"/>
-      <c r="H37" s="59"/>
+      <c r="E37" s="77"/>
+      <c r="F37" s="77"/>
+      <c r="G37" s="77"/>
+      <c r="H37" s="77"/>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="61" t="s">
+      <c r="A38" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="61"/>
-      <c r="C38" s="62"/>
-      <c r="D38" s="63"/>
-      <c r="E38" s="63"/>
-      <c r="F38" s="63"/>
-      <c r="G38" s="63"/>
-      <c r="H38" s="64"/>
+      <c r="B38" s="39"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="41"/>
+      <c r="H38" s="42"/>
       <c r="I38" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="J38" s="48"/>
-      <c r="K38" s="48"/>
-      <c r="L38" s="82"/>
-      <c r="M38" s="82"/>
-      <c r="N38" s="83"/>
+      <c r="J38" s="72"/>
+      <c r="K38" s="72"/>
+      <c r="L38" s="58"/>
+      <c r="M38" s="58"/>
+      <c r="N38" s="59"/>
     </row>
     <row r="39" spans="1:14" ht="3.75" customHeight="1">
       <c r="J39" s="19"/>
     </row>
     <row r="40" spans="1:14">
-      <c r="A40" s="78" t="s">
+      <c r="A40" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="78"/>
-      <c r="C40" s="78"/>
-      <c r="D40" s="78"/>
-      <c r="E40" s="78"/>
-      <c r="F40" s="78"/>
-      <c r="G40" s="78"/>
-      <c r="H40" s="78" t="s">
+      <c r="B40" s="54"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="54"/>
+      <c r="E40" s="54"/>
+      <c r="F40" s="54"/>
+      <c r="G40" s="54"/>
+      <c r="H40" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="I40" s="78"/>
-      <c r="J40" s="78"/>
-      <c r="K40" s="78"/>
-      <c r="L40" s="78" t="s">
+      <c r="I40" s="54"/>
+      <c r="J40" s="54"/>
+      <c r="K40" s="54"/>
+      <c r="L40" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="M40" s="78"/>
-      <c r="N40" s="78"/>
+      <c r="M40" s="54"/>
+      <c r="N40" s="54"/>
     </row>
     <row r="41" spans="1:14">
-      <c r="A41" s="77"/>
-      <c r="B41" s="77"/>
-      <c r="C41" s="77"/>
-      <c r="D41" s="77"/>
-      <c r="E41" s="77"/>
-      <c r="F41" s="77"/>
-      <c r="G41" s="77"/>
-      <c r="H41" s="77"/>
-      <c r="I41" s="77"/>
-      <c r="J41" s="77"/>
-      <c r="K41" s="77"/>
-      <c r="L41" s="79"/>
-      <c r="M41" s="79"/>
-      <c r="N41" s="79"/>
+      <c r="A41" s="53"/>
+      <c r="B41" s="53"/>
+      <c r="C41" s="53"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="53"/>
+      <c r="F41" s="53"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="53"/>
+      <c r="I41" s="53"/>
+      <c r="J41" s="53"/>
+      <c r="K41" s="53"/>
+      <c r="L41" s="55"/>
+      <c r="M41" s="55"/>
+      <c r="N41" s="55"/>
     </row>
     <row r="42" spans="1:14">
-      <c r="A42" s="77"/>
-      <c r="B42" s="77"/>
-      <c r="C42" s="77"/>
-      <c r="D42" s="77"/>
-      <c r="E42" s="77"/>
-      <c r="F42" s="77"/>
-      <c r="G42" s="77"/>
-      <c r="H42" s="77"/>
-      <c r="I42" s="77"/>
-      <c r="J42" s="77"/>
-      <c r="K42" s="77"/>
-      <c r="L42" s="79"/>
-      <c r="M42" s="79"/>
-      <c r="N42" s="79"/>
+      <c r="A42" s="53"/>
+      <c r="B42" s="53"/>
+      <c r="C42" s="53"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="53"/>
+      <c r="F42" s="53"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="53"/>
+      <c r="I42" s="53"/>
+      <c r="J42" s="53"/>
+      <c r="K42" s="53"/>
+      <c r="L42" s="55"/>
+      <c r="M42" s="55"/>
+      <c r="N42" s="55"/>
     </row>
     <row r="43" spans="1:14">
-      <c r="A43" s="77"/>
-      <c r="B43" s="77"/>
-      <c r="C43" s="77"/>
-      <c r="D43" s="77"/>
-      <c r="E43" s="77"/>
-      <c r="F43" s="77"/>
-      <c r="G43" s="77"/>
-      <c r="H43" s="77"/>
-      <c r="I43" s="77"/>
-      <c r="J43" s="77"/>
-      <c r="K43" s="77"/>
-      <c r="L43" s="79"/>
-      <c r="M43" s="79"/>
-      <c r="N43" s="79"/>
+      <c r="A43" s="53"/>
+      <c r="B43" s="53"/>
+      <c r="C43" s="53"/>
+      <c r="D43" s="53"/>
+      <c r="E43" s="53"/>
+      <c r="F43" s="53"/>
+      <c r="G43" s="53"/>
+      <c r="H43" s="53"/>
+      <c r="I43" s="53"/>
+      <c r="J43" s="53"/>
+      <c r="K43" s="53"/>
+      <c r="L43" s="55"/>
+      <c r="M43" s="55"/>
+      <c r="N43" s="55"/>
     </row>
     <row r="44" spans="1:14">
-      <c r="A44" s="77"/>
-      <c r="B44" s="77"/>
-      <c r="C44" s="77"/>
-      <c r="D44" s="77"/>
-      <c r="E44" s="77"/>
-      <c r="F44" s="77"/>
-      <c r="G44" s="77"/>
-      <c r="H44" s="77"/>
-      <c r="I44" s="77"/>
-      <c r="J44" s="77"/>
-      <c r="K44" s="77"/>
-      <c r="L44" s="79"/>
-      <c r="M44" s="79"/>
-      <c r="N44" s="79"/>
+      <c r="A44" s="53"/>
+      <c r="B44" s="53"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="53"/>
+      <c r="K44" s="53"/>
+      <c r="L44" s="55"/>
+      <c r="M44" s="55"/>
+      <c r="N44" s="55"/>
     </row>
     <row r="45" spans="1:14" ht="3.75" customHeight="1"/>
     <row r="46" spans="1:14">
-      <c r="A46" s="80" t="s">
+      <c r="A46" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="81"/>
-      <c r="C46" s="73"/>
-      <c r="D46" s="73"/>
-      <c r="E46" s="73"/>
-      <c r="F46" s="73"/>
-      <c r="G46" s="73"/>
-      <c r="H46" s="73"/>
-      <c r="I46" s="73"/>
-      <c r="J46" s="73"/>
-      <c r="K46" s="74"/>
-      <c r="L46" s="65"/>
-      <c r="M46" s="66"/>
-      <c r="N46" s="67"/>
+      <c r="B46" s="57"/>
+      <c r="C46" s="49"/>
+      <c r="D46" s="49"/>
+      <c r="E46" s="49"/>
+      <c r="F46" s="49"/>
+      <c r="G46" s="49"/>
+      <c r="H46" s="49"/>
+      <c r="I46" s="49"/>
+      <c r="J46" s="49"/>
+      <c r="K46" s="50"/>
+      <c r="L46" s="43"/>
+      <c r="M46" s="44"/>
+      <c r="N46" s="45"/>
     </row>
     <row r="47" spans="1:14" ht="15" customHeight="1">
       <c r="A47" s="14"/>
       <c r="B47" s="15"/>
-      <c r="C47" s="75"/>
-      <c r="D47" s="75"/>
-      <c r="E47" s="75"/>
-      <c r="F47" s="75"/>
-      <c r="G47" s="75"/>
-      <c r="H47" s="75"/>
-      <c r="I47" s="75"/>
-      <c r="J47" s="75"/>
-      <c r="K47" s="76"/>
+      <c r="C47" s="51"/>
+      <c r="D47" s="51"/>
+      <c r="E47" s="51"/>
+      <c r="F47" s="51"/>
+      <c r="G47" s="51"/>
+      <c r="H47" s="51"/>
+      <c r="I47" s="51"/>
+      <c r="J47" s="51"/>
+      <c r="K47" s="52"/>
       <c r="L47" s="14"/>
       <c r="M47" s="15"/>
       <c r="N47" s="16"/>
@@ -1889,19 +1892,19 @@
       <c r="C50" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D50" s="69"/>
-      <c r="E50" s="69"/>
-      <c r="F50" s="69"/>
-      <c r="G50" s="69"/>
-      <c r="H50" s="69"/>
-      <c r="I50" s="69"/>
-      <c r="J50" s="69"/>
-      <c r="K50" s="70"/>
-      <c r="L50" s="68" t="s">
+      <c r="D50" s="47"/>
+      <c r="E50" s="47"/>
+      <c r="F50" s="47"/>
+      <c r="G50" s="47"/>
+      <c r="H50" s="47"/>
+      <c r="I50" s="47"/>
+      <c r="J50" s="47"/>
+      <c r="K50" s="48"/>
+      <c r="L50" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="M50" s="68"/>
-      <c r="N50" s="68"/>
+      <c r="M50" s="46"/>
+      <c r="N50" s="46"/>
       <c r="O50" s="11"/>
     </row>
     <row r="51" spans="1:15">
@@ -1912,17 +1915,17 @@
       <c r="C51" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D51" s="71"/>
-      <c r="E51" s="71"/>
-      <c r="F51" s="71"/>
-      <c r="G51" s="71"/>
-      <c r="H51" s="71"/>
-      <c r="I51" s="71"/>
-      <c r="J51" s="71"/>
-      <c r="K51" s="72"/>
-      <c r="L51" s="68"/>
-      <c r="M51" s="68"/>
-      <c r="N51" s="68"/>
+      <c r="D51" s="83"/>
+      <c r="E51" s="83"/>
+      <c r="F51" s="83"/>
+      <c r="G51" s="83"/>
+      <c r="H51" s="83"/>
+      <c r="I51" s="83"/>
+      <c r="J51" s="83"/>
+      <c r="K51" s="84"/>
+      <c r="L51" s="46"/>
+      <c r="M51" s="46"/>
+      <c r="N51" s="46"/>
     </row>
     <row r="52" spans="1:15" ht="15" customHeight="1">
       <c r="A52" s="31" t="s">
@@ -1932,160 +1935,224 @@
       <c r="C52" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D52" s="57"/>
-      <c r="E52" s="57"/>
-      <c r="F52" s="57"/>
-      <c r="G52" s="57"/>
-      <c r="H52" s="57"/>
-      <c r="I52" s="57"/>
-      <c r="J52" s="57"/>
-      <c r="K52" s="58"/>
+      <c r="D52" s="66"/>
+      <c r="E52" s="66"/>
+      <c r="F52" s="66"/>
+      <c r="G52" s="66"/>
+      <c r="H52" s="66"/>
+      <c r="I52" s="66"/>
+      <c r="J52" s="66"/>
+      <c r="K52" s="67"/>
     </row>
     <row r="53" spans="1:15" ht="4.5" customHeight="1"/>
     <row r="54" spans="1:15">
-      <c r="A54" s="56" t="s">
+      <c r="A54" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="B54" s="56"/>
+      <c r="B54" s="68"/>
       <c r="C54" s="10"/>
-      <c r="D54" s="56" t="s">
+      <c r="D54" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="E54" s="56"/>
-      <c r="F54" s="56"/>
-      <c r="G54" s="56"/>
-      <c r="H54" s="56"/>
-      <c r="I54" s="56"/>
+      <c r="E54" s="68"/>
+      <c r="F54" s="68"/>
+      <c r="G54" s="68"/>
+      <c r="H54" s="68"/>
+      <c r="I54" s="68"/>
       <c r="J54" s="10"/>
-      <c r="K54" s="56" t="s">
+      <c r="K54" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="L54" s="56"/>
-      <c r="M54" s="56"/>
-      <c r="N54" s="56"/>
+      <c r="L54" s="68"/>
+      <c r="M54" s="68"/>
+      <c r="N54" s="68"/>
     </row>
     <row r="55" spans="1:15">
-      <c r="A55" s="56" t="s">
+      <c r="A55" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="B55" s="56"/>
+      <c r="B55" s="68"/>
       <c r="C55" s="10"/>
-      <c r="D55" s="56" t="s">
+      <c r="D55" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="E55" s="56"/>
-      <c r="F55" s="56" t="s">
+      <c r="E55" s="68"/>
+      <c r="F55" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="G55" s="56"/>
-      <c r="H55" s="56" t="s">
+      <c r="G55" s="68"/>
+      <c r="H55" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="I55" s="56"/>
+      <c r="I55" s="68"/>
       <c r="J55" s="25"/>
-      <c r="K55" s="56" t="s">
+      <c r="K55" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="L55" s="56"/>
-      <c r="M55" s="56" t="s">
+      <c r="L55" s="68"/>
+      <c r="M55" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="N55" s="56"/>
+      <c r="N55" s="68"/>
     </row>
     <row r="56" spans="1:15">
-      <c r="A56" s="56"/>
-      <c r="B56" s="56"/>
+      <c r="A56" s="68"/>
+      <c r="B56" s="68"/>
       <c r="C56" s="10"/>
-      <c r="D56" s="56"/>
-      <c r="E56" s="56"/>
-      <c r="F56" s="56"/>
-      <c r="G56" s="56"/>
-      <c r="H56" s="56"/>
-      <c r="I56" s="56"/>
+      <c r="D56" s="68"/>
+      <c r="E56" s="68"/>
+      <c r="F56" s="68"/>
+      <c r="G56" s="68"/>
+      <c r="H56" s="68"/>
+      <c r="I56" s="68"/>
       <c r="J56" s="10"/>
-      <c r="K56" s="56"/>
-      <c r="L56" s="56"/>
-      <c r="M56" s="56"/>
-      <c r="N56" s="56"/>
+      <c r="K56" s="68"/>
+      <c r="L56" s="68"/>
+      <c r="M56" s="68"/>
+      <c r="N56" s="68"/>
     </row>
     <row r="57" spans="1:15">
-      <c r="A57" s="56"/>
-      <c r="B57" s="56"/>
+      <c r="A57" s="68"/>
+      <c r="B57" s="68"/>
       <c r="C57" s="10"/>
-      <c r="D57" s="56"/>
-      <c r="E57" s="56"/>
-      <c r="F57" s="56"/>
-      <c r="G57" s="56"/>
-      <c r="H57" s="56"/>
-      <c r="I57" s="56"/>
+      <c r="D57" s="68"/>
+      <c r="E57" s="68"/>
+      <c r="F57" s="68"/>
+      <c r="G57" s="68"/>
+      <c r="H57" s="68"/>
+      <c r="I57" s="68"/>
       <c r="J57" s="10"/>
-      <c r="K57" s="56"/>
-      <c r="L57" s="56"/>
-      <c r="M57" s="56"/>
-      <c r="N57" s="56"/>
+      <c r="K57" s="68"/>
+      <c r="L57" s="68"/>
+      <c r="M57" s="68"/>
+      <c r="N57" s="68"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="56"/>
-      <c r="B58" s="56"/>
+      <c r="A58" s="68"/>
+      <c r="B58" s="68"/>
       <c r="C58" s="10"/>
-      <c r="D58" s="56"/>
-      <c r="E58" s="56"/>
-      <c r="F58" s="56"/>
-      <c r="G58" s="56"/>
-      <c r="H58" s="56"/>
-      <c r="I58" s="56"/>
+      <c r="D58" s="68"/>
+      <c r="E58" s="68"/>
+      <c r="F58" s="68"/>
+      <c r="G58" s="68"/>
+      <c r="H58" s="68"/>
+      <c r="I58" s="68"/>
       <c r="J58" s="10"/>
-      <c r="K58" s="56"/>
-      <c r="L58" s="56"/>
-      <c r="M58" s="56"/>
-      <c r="N58" s="56"/>
+      <c r="K58" s="68"/>
+      <c r="L58" s="68"/>
+      <c r="M58" s="68"/>
+      <c r="N58" s="68"/>
     </row>
     <row r="59" spans="1:15">
-      <c r="A59" s="56"/>
-      <c r="B59" s="56"/>
+      <c r="A59" s="68"/>
+      <c r="B59" s="68"/>
       <c r="C59" s="10"/>
-      <c r="D59" s="56"/>
-      <c r="E59" s="56"/>
-      <c r="F59" s="56"/>
-      <c r="G59" s="56"/>
-      <c r="H59" s="56"/>
-      <c r="I59" s="56"/>
+      <c r="D59" s="68"/>
+      <c r="E59" s="68"/>
+      <c r="F59" s="68"/>
+      <c r="G59" s="68"/>
+      <c r="H59" s="68"/>
+      <c r="I59" s="68"/>
       <c r="J59" s="10"/>
-      <c r="K59" s="56"/>
-      <c r="L59" s="56"/>
-      <c r="M59" s="56"/>
-      <c r="N59" s="56"/>
+      <c r="K59" s="68"/>
+      <c r="L59" s="68"/>
+      <c r="M59" s="68"/>
+      <c r="N59" s="68"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="56" t="s">
+      <c r="A60" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="56"/>
+      <c r="B60" s="68"/>
       <c r="C60" s="10"/>
-      <c r="D60" s="56" t="s">
+      <c r="D60" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="E60" s="56"/>
-      <c r="F60" s="56" t="s">
+      <c r="E60" s="68"/>
+      <c r="F60" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="G60" s="56"/>
-      <c r="H60" s="56" t="s">
+      <c r="G60" s="68"/>
+      <c r="H60" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="I60" s="56"/>
+      <c r="I60" s="68"/>
       <c r="J60" s="10"/>
-      <c r="K60" s="56" t="s">
+      <c r="K60" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="L60" s="56"/>
-      <c r="M60" s="56" t="s">
+      <c r="L60" s="68"/>
+      <c r="M60" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="N60" s="56"/>
+      <c r="N60" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="80">
+    <mergeCell ref="Q3:S4"/>
+    <mergeCell ref="Q6:S7"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="I7:N8"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="F15:G17"/>
+    <mergeCell ref="H15:K17"/>
+    <mergeCell ref="L15:N17"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E17"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="L18:N18"/>
+    <mergeCell ref="K22:N22"/>
+    <mergeCell ref="D19:N21"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="C23:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="E35:H35"/>
+    <mergeCell ref="E36:H36"/>
+    <mergeCell ref="K34:N34"/>
+    <mergeCell ref="K35:N35"/>
+    <mergeCell ref="K25:N25"/>
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="K27:N27"/>
+    <mergeCell ref="K23:N24"/>
+    <mergeCell ref="E37:H37"/>
+    <mergeCell ref="M56:N59"/>
+    <mergeCell ref="K60:L60"/>
+    <mergeCell ref="M60:N60"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="D52:K52"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A56:B59"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="K54:N54"/>
+    <mergeCell ref="D54:I54"/>
+    <mergeCell ref="M55:N55"/>
+    <mergeCell ref="D56:E59"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="F56:G59"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="H56:I59"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="K56:L59"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B26"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="D12:K12"/>
+    <mergeCell ref="D11:K11"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:H38"/>
     <mergeCell ref="L46:N46"/>
@@ -2102,70 +2169,6 @@
     <mergeCell ref="A40:G40"/>
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="L38:N38"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="D12:K12"/>
-    <mergeCell ref="D11:K11"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B26"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D52:K52"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A56:B59"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="K54:N54"/>
-    <mergeCell ref="D54:I54"/>
-    <mergeCell ref="M55:N55"/>
-    <mergeCell ref="D56:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="F56:G59"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="H56:I59"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="K56:L59"/>
-    <mergeCell ref="M56:N59"/>
-    <mergeCell ref="K60:L60"/>
-    <mergeCell ref="M60:N60"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="L18:N18"/>
-    <mergeCell ref="K22:N22"/>
-    <mergeCell ref="D19:N21"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="C23:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="E35:H35"/>
-    <mergeCell ref="E36:H36"/>
-    <mergeCell ref="K34:N34"/>
-    <mergeCell ref="K35:N35"/>
-    <mergeCell ref="K25:N25"/>
-    <mergeCell ref="K26:N26"/>
-    <mergeCell ref="K27:N27"/>
-    <mergeCell ref="K23:N24"/>
-    <mergeCell ref="E37:H37"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="F15:G17"/>
-    <mergeCell ref="H15:K17"/>
-    <mergeCell ref="L15:N17"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E17"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="Q3:S4"/>
-    <mergeCell ref="Q6:S7"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="I7:N8"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0" bottom="0" header="0" footer="0.3"/>

</xml_diff>